<commit_message>
Testing Sprint2. Sprint2 ultimato
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
+++ b/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\LORI\UNIVERSITA'\Magistrale\2°Anno\II Ciclo\Ingegneria dei Sistemi Software\Waiter_Robot\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F325D139-8EF2-4512-980B-AD530E9F9CC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2CF017-57EC-415A-9C2C-8A76D81C18BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
   <si>
     <t>Sprint Goal (obiettivo)</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>CONCLUSO</t>
-  </si>
-  <si>
-    <t>Revisione del progetto</t>
   </si>
   <si>
     <t>Pianificazione di un test plan</t>
@@ -733,10 +730,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,66 +755,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -817,64 +820,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -886,32 +892,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,7 +949,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3836895</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1213,13 +1210,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3840480</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1301,13 +1298,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3840480</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1488,7 +1485,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="it-IT" sz="1100" b="0" baseline="0"/>
-            <a:t>-meno costi comporterà</a:t>
+            <a:t>-meno costi comporterà.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1818,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD0328D-D609-42F7-8061-4CD2A9785B96}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1831,13 +1828,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1845,19 +1842,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="68"/>
       <c r="B3" s="67" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1865,10 +1862,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1876,10 +1873,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1887,10 +1884,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1898,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1906,7 +1903,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1914,7 +1911,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1922,7 +1919,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1930,7 +1927,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1938,7 +1935,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1946,7 +1943,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1954,7 +1951,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1962,7 +1959,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1970,7 +1967,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1994,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6357E3-4FBB-418C-9BB3-004C68F042FF}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96:G106"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,51 +2011,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
+      <c r="A1" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
     </row>
     <row r="3" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A3" s="69"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="129"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="105"/>
     </row>
     <row r="4" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A4" s="69"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="129"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="105"/>
     </row>
     <row r="5" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A5" s="69"/>
-      <c r="B5" s="124"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="126"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="108"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
@@ -2071,7 +2068,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>4</v>
@@ -2082,27 +2079,27 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="92" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="54"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="70" t="s">
+      <c r="G7" s="92" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="70"/>
-      <c r="B8" s="103"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
@@ -2111,13 +2108,13 @@
       <c r="F8" s="11">
         <v>44002</v>
       </c>
-      <c r="G8" s="70"/>
+      <c r="G8" s="92"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" s="70"/>
-      <c r="B9" s="104"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
@@ -2126,13 +2123,13 @@
       <c r="F9" s="11">
         <v>44003</v>
       </c>
-      <c r="G9" s="70"/>
+      <c r="G9" s="92"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="70"/>
-      <c r="B10" s="104"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="s">
@@ -2141,13 +2138,13 @@
       <c r="F10" s="11">
         <v>44004</v>
       </c>
-      <c r="G10" s="70"/>
+      <c r="G10" s="92"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
-      <c r="B11" s="105"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="96"/>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
@@ -2156,1152 +2153,1175 @@
       <c r="F11" s="65">
         <v>44005</v>
       </c>
-      <c r="G11" s="70"/>
+      <c r="G11" s="92"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="71">
+      <c r="A12" s="85">
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="85" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
-      <c r="B13" s="100" t="s">
-        <v>37</v>
+      <c r="A13" s="85"/>
+      <c r="B13" s="80" t="s">
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="95"/>
+        <v>23</v>
+      </c>
+      <c r="D13" s="97"/>
       <c r="E13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="11">
         <v>44006</v>
       </c>
-      <c r="G13" s="71"/>
+      <c r="G13" s="85"/>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
-      <c r="B14" s="101"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="96"/>
+        <v>44</v>
+      </c>
+      <c r="D14" s="98"/>
       <c r="E14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="11">
         <v>44007</v>
       </c>
-      <c r="G14" s="71"/>
+      <c r="G14" s="85"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="B15" s="101"/>
+      <c r="A15" s="85"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="96"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="98"/>
       <c r="E15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="11">
         <v>44007</v>
       </c>
-      <c r="G15" s="71"/>
+      <c r="G15" s="85"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
-      <c r="B16" s="101"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="96"/>
+        <v>25</v>
+      </c>
+      <c r="D16" s="98"/>
       <c r="E16" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="71"/>
+      <c r="G16" s="85"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="71"/>
-      <c r="B17" s="101"/>
+      <c r="A17" s="85"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="96"/>
+        <v>42</v>
+      </c>
+      <c r="D17" s="98"/>
       <c r="E17" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="11">
         <v>44009</v>
       </c>
-      <c r="G17" s="71"/>
+      <c r="G17" s="85"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="71"/>
-      <c r="B18" s="101"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="96"/>
+        <v>50</v>
+      </c>
+      <c r="D18" s="98"/>
       <c r="E18" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="11">
         <v>44009</v>
       </c>
-      <c r="G18" s="71"/>
+      <c r="G18" s="85"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
-      <c r="B19" s="101"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="83"/>
       <c r="C19" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="96"/>
+        <v>43</v>
+      </c>
+      <c r="D19" s="98"/>
       <c r="E19" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="11">
         <v>44009</v>
       </c>
-      <c r="G19" s="71"/>
+      <c r="G19" s="85"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="71"/>
-      <c r="B20" s="102"/>
+      <c r="A20" s="85"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="96"/>
+        <v>24</v>
+      </c>
+      <c r="D20" s="98"/>
       <c r="E20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="11">
         <v>44009</v>
       </c>
-      <c r="G20" s="71"/>
+      <c r="G20" s="85"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="71"/>
+      <c r="A21" s="85"/>
       <c r="B21" s="50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="71"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16">
+        <v>44016</v>
+      </c>
+      <c r="G21" s="85"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="71"/>
+      <c r="A22" s="85"/>
       <c r="B22" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="71"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
+        <v>44016</v>
+      </c>
+      <c r="G22" s="85"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="88">
+      <c r="A23" s="84">
         <v>2</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="55"/>
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
-      <c r="G23" s="88"/>
+      <c r="G23" s="84" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="88"/>
-      <c r="B24" s="100" t="s">
-        <v>37</v>
+      <c r="A24" s="84"/>
+      <c r="B24" s="80" t="s">
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="95"/>
-      <c r="E24" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D24" s="97"/>
+      <c r="E24" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F24" s="16">
         <v>44010</v>
       </c>
-      <c r="G24" s="88"/>
+      <c r="G24" s="84"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
-      <c r="B25" s="101"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="83"/>
       <c r="C25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="96"/>
-      <c r="E25" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="D25" s="98"/>
+      <c r="E25" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F25" s="16">
         <v>44012</v>
       </c>
-      <c r="G25" s="88"/>
+      <c r="G25" s="84"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="88"/>
-      <c r="B26" s="101"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="83"/>
       <c r="C26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="96"/>
-      <c r="E26" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="D26" s="98"/>
+      <c r="E26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F26" s="16">
         <v>44012</v>
       </c>
-      <c r="G26" s="88"/>
+      <c r="G26" s="84"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="88"/>
-      <c r="B27" s="101"/>
+      <c r="A27" s="84"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="98"/>
+      <c r="E27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="84"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A28" s="84"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="96"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="88"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="88"/>
-      <c r="B28" s="101"/>
-      <c r="C28" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="96"/>
-      <c r="E28" s="4"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F28" s="16">
         <v>44013</v>
       </c>
-      <c r="G28" s="88"/>
+      <c r="G28" s="84"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="88"/>
-      <c r="B29" s="101"/>
+      <c r="A29" s="84"/>
+      <c r="B29" s="83"/>
       <c r="C29" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="96"/>
-      <c r="E29" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="D29" s="98"/>
+      <c r="E29" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F29" s="16">
         <v>44015</v>
       </c>
-      <c r="G29" s="88"/>
+      <c r="G29" s="84"/>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="88"/>
-      <c r="B30" s="101"/>
+      <c r="A30" s="84"/>
+      <c r="B30" s="83"/>
       <c r="C30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="96"/>
-      <c r="E30" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D30" s="98"/>
+      <c r="E30" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F30" s="16">
         <v>44016</v>
       </c>
-      <c r="G30" s="88"/>
+      <c r="G30" s="84"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="88"/>
-      <c r="B31" s="102"/>
-      <c r="D31" s="96"/>
-      <c r="E31" s="4"/>
-      <c r="G31" s="88"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="16">
+        <v>44016</v>
+      </c>
+      <c r="G31" s="84"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="88"/>
-      <c r="B32" s="60" t="s">
-        <v>39</v>
+      <c r="A32" s="84"/>
+      <c r="B32" s="50" t="s">
+        <v>8</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="88"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="88"/>
-      <c r="B33" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="88"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="99">
+      <c r="D32" s="99"/>
+      <c r="E32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="16">
+        <v>44016</v>
+      </c>
+      <c r="G32" s="84"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="93">
         <v>3</v>
       </c>
-      <c r="B34" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="72"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="99"/>
-      <c r="B35" s="100" t="s">
-        <v>37</v>
-      </c>
+      <c r="B33" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="76"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="93"/>
+      <c r="B34" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="121" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="77"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A35" s="93"/>
+      <c r="B35" s="83"/>
       <c r="C35" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="118" t="s">
-        <v>62</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D35" s="122"/>
       <c r="E35" s="4"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="73"/>
+      <c r="G35" s="77"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="99"/>
-      <c r="B36" s="101"/>
+      <c r="A36" s="93"/>
+      <c r="B36" s="83"/>
       <c r="C36" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="119"/>
+        <v>11</v>
+      </c>
+      <c r="D36" s="122"/>
       <c r="E36" s="4"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="73"/>
+      <c r="G36" s="77"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="99"/>
-      <c r="B37" s="101"/>
-      <c r="C37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="119"/>
+      <c r="A37" s="93"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="122"/>
       <c r="E37" s="4"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="73"/>
+      <c r="G37" s="77"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="99"/>
-      <c r="B38" s="101"/>
-      <c r="C38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="119"/>
+      <c r="A38" s="93"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="122"/>
       <c r="E38" s="4"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="73"/>
+      <c r="G38" s="77"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="99"/>
-      <c r="B39" s="101"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="119"/>
+      <c r="A39" s="93"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="122"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="73"/>
+      <c r="F39" s="16">
+        <v>44018</v>
+      </c>
+      <c r="G39" s="77"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="99"/>
-      <c r="B40" s="102"/>
-      <c r="C40" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="119"/>
+      <c r="A40" s="93"/>
+      <c r="B40" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="64"/>
+      <c r="D40" s="122"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="16">
-        <v>44018</v>
-      </c>
-      <c r="G40" s="73"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="77"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="99"/>
+      <c r="A41" s="93"/>
       <c r="B41" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="119"/>
+        <v>8</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="123"/>
       <c r="E41" s="4"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="73"/>
-    </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="99"/>
-      <c r="B42" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="120"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="74"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="106">
+      <c r="G41" s="78"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="86">
         <v>4</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="75"/>
+      <c r="B42" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="26"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="124"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A43" s="86"/>
+      <c r="B43" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="125"/>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="106"/>
-      <c r="B44" s="81" t="s">
-        <v>37</v>
-      </c>
+      <c r="A44" s="86"/>
+      <c r="B44" s="79"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="4"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="76"/>
+      <c r="G44" s="125"/>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="106"/>
-      <c r="B45" s="81"/>
+      <c r="A45" s="86"/>
+      <c r="B45" s="79"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="4"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="76"/>
+      <c r="G45" s="125"/>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="106"/>
-      <c r="B46" s="81"/>
+      <c r="A46" s="86"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="4"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="76"/>
+      <c r="G46" s="125"/>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="106"/>
-      <c r="B47" s="81"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="A47" s="86"/>
+      <c r="B47" s="79"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
       <c r="E47" s="4"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="76"/>
+      <c r="F47" s="16">
+        <v>44022</v>
+      </c>
+      <c r="G47" s="125"/>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="106"/>
-      <c r="B48" s="81"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
+      <c r="A48" s="86"/>
+      <c r="B48" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
       <c r="E48" s="4"/>
-      <c r="F48" s="16">
-        <v>44022</v>
-      </c>
-      <c r="G48" s="76"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="125"/>
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="106"/>
+      <c r="A49" s="86"/>
       <c r="B49" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="4"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="76"/>
-    </row>
-    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" s="106"/>
-      <c r="B50" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="77"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="107">
+      <c r="G49" s="126"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="87">
         <v>5</v>
       </c>
-      <c r="B51" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="30" t="s">
+      <c r="B50" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="30"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="127"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A51" s="87"/>
+      <c r="B51" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="128"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A52" s="87"/>
+      <c r="B52" s="79"/>
+      <c r="C52" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D51" s="30"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="78"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="107"/>
-      <c r="B52" s="81" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="4"/>
       <c r="F52" s="16"/>
-      <c r="G52" s="79"/>
+      <c r="G52" s="128"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="107"/>
-      <c r="B53" s="81"/>
+      <c r="A53" s="87"/>
+      <c r="B53" s="79"/>
       <c r="C53" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="4"/>
       <c r="F53" s="16"/>
-      <c r="G53" s="79"/>
+      <c r="G53" s="128"/>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="107"/>
-      <c r="B54" s="81"/>
-      <c r="C54" s="2" t="s">
-        <v>12</v>
+      <c r="A54" s="87"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="4"/>
       <c r="F54" s="16"/>
-      <c r="G54" s="79"/>
+      <c r="G54" s="128"/>
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="107"/>
-      <c r="B55" s="81"/>
-      <c r="C55" s="1" t="s">
-        <v>26</v>
+      <c r="A55" s="87"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="79"/>
+      <c r="F55" s="16">
+        <v>44026</v>
+      </c>
+      <c r="G55" s="128"/>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="107"/>
-      <c r="B56" s="81"/>
-      <c r="C56" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A56" s="87"/>
+      <c r="B56" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="5"/>
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="16">
-        <v>44026</v>
-      </c>
-      <c r="G56" s="79"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="128"/>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="107"/>
+      <c r="A57" s="87"/>
       <c r="B57" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="79"/>
-    </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A58" s="107"/>
-      <c r="B58" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="80"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="108">
+      <c r="G57" s="129"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="88">
         <v>6</v>
       </c>
-      <c r="B59" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" s="49"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="89"/>
+      <c r="B58" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="49"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="115"/>
+    </row>
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A59" s="88"/>
+      <c r="B59" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="116"/>
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" s="108"/>
-      <c r="B60" s="81" t="s">
-        <v>37</v>
-      </c>
+      <c r="A60" s="88"/>
+      <c r="B60" s="79"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="4"/>
       <c r="F60" s="16"/>
-      <c r="G60" s="90"/>
+      <c r="G60" s="116"/>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" s="108"/>
-      <c r="B61" s="81"/>
+      <c r="A61" s="88"/>
+      <c r="B61" s="79"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="4"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="90"/>
+      <c r="G61" s="116"/>
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A62" s="108"/>
-      <c r="B62" s="81"/>
+      <c r="A62" s="88"/>
+      <c r="B62" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="4"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="90"/>
+      <c r="G62" s="116"/>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="108"/>
+      <c r="A63" s="88"/>
       <c r="B63" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="4"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="90"/>
-    </row>
-    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" s="108"/>
-      <c r="B64" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="91"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="109">
+      <c r="G63" s="117"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="89">
         <v>6</v>
       </c>
-      <c r="B65" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="92"/>
+      <c r="B64" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="118"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A65" s="89"/>
+      <c r="B65" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="119"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="109"/>
-      <c r="B66" s="81" t="s">
-        <v>37</v>
-      </c>
+      <c r="A66" s="89"/>
+      <c r="B66" s="79"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="4"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="93"/>
+      <c r="G66" s="119"/>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A67" s="109"/>
-      <c r="B67" s="81"/>
+      <c r="A67" s="89"/>
+      <c r="B67" s="79"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="4"/>
       <c r="F67" s="16"/>
-      <c r="G67" s="93"/>
+      <c r="G67" s="119"/>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A68" s="109"/>
-      <c r="B68" s="81"/>
+      <c r="A68" s="89"/>
+      <c r="B68" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="4"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="93"/>
+      <c r="G68" s="119"/>
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="109"/>
+      <c r="A69" s="89"/>
       <c r="B69" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="4"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="93"/>
-    </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A70" s="109"/>
-      <c r="B70" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="94"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="110">
+      <c r="G69" s="120"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="90">
         <v>7</v>
       </c>
-      <c r="B71" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="40"/>
-      <c r="F71" s="41"/>
-      <c r="G71" s="85"/>
+      <c r="B70" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="40"/>
+      <c r="F70" s="41"/>
+      <c r="G70" s="112"/>
+    </row>
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A71" s="90"/>
+      <c r="B71" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="113"/>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="110"/>
-      <c r="B72" s="81" t="s">
-        <v>37</v>
-      </c>
+      <c r="A72" s="90"/>
+      <c r="B72" s="79"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="4"/>
       <c r="F72" s="16"/>
-      <c r="G72" s="86"/>
+      <c r="G72" s="113"/>
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A73" s="110"/>
-      <c r="B73" s="81"/>
+      <c r="A73" s="90"/>
+      <c r="B73" s="79"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="4"/>
       <c r="F73" s="16"/>
-      <c r="G73" s="86"/>
+      <c r="G73" s="113"/>
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A74" s="110"/>
-      <c r="B74" s="81"/>
+      <c r="A74" s="90"/>
+      <c r="B74" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="4"/>
       <c r="F74" s="16"/>
-      <c r="G74" s="86"/>
+      <c r="G74" s="113"/>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A75" s="110"/>
+      <c r="A75" s="90"/>
       <c r="B75" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="4"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="86"/>
-    </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A76" s="110"/>
-      <c r="B76" s="50" t="s">
+      <c r="G75" s="114"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="82">
         <v>8</v>
       </c>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="16"/>
-      <c r="G76" s="87"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="111">
-        <v>8</v>
-      </c>
-      <c r="B77" s="42" t="s">
+      <c r="B76" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="43"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="82"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="109"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A77" s="82"/>
+      <c r="B77" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="110"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A78" s="111"/>
-      <c r="B78" s="81" t="s">
-        <v>37</v>
-      </c>
+      <c r="A78" s="82"/>
+      <c r="B78" s="79"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="4"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="83"/>
+      <c r="G78" s="110"/>
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A79" s="111"/>
-      <c r="B79" s="81"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="50" t="s">
+        <v>7</v>
+      </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="4"/>
       <c r="F79" s="16"/>
-      <c r="G79" s="83"/>
+      <c r="G79" s="110"/>
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A80" s="111"/>
+      <c r="A80" s="82"/>
       <c r="B80" s="50" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="4"/>
       <c r="F80" s="16"/>
-      <c r="G80" s="83"/>
+      <c r="G80" s="110"/>
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A81" s="111"/>
+      <c r="A81" s="82"/>
       <c r="B81" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="4"/>
       <c r="F81" s="16"/>
-      <c r="G81" s="83"/>
-    </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A82" s="111"/>
-      <c r="B82" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="84"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="71">
+      <c r="G81" s="111"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="85">
         <v>9</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B82" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="112"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="70"/>
+    </row>
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A83" s="85"/>
+      <c r="B83" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="71"/>
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A84" s="71"/>
-      <c r="B84" s="81" t="s">
-        <v>37</v>
-      </c>
+      <c r="A84" s="85"/>
+      <c r="B84" s="79"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="4"/>
       <c r="F84" s="16"/>
-      <c r="G84" s="113"/>
+      <c r="G84" s="71"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A85" s="71"/>
-      <c r="B85" s="81"/>
+      <c r="A85" s="85"/>
+      <c r="B85" s="79"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="4"/>
       <c r="F85" s="16"/>
-      <c r="G85" s="113"/>
+      <c r="G85" s="71"/>
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A86" s="71"/>
-      <c r="B86" s="81"/>
+      <c r="A86" s="85"/>
+      <c r="B86" s="50" t="s">
+        <v>7</v>
+      </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="4"/>
       <c r="F86" s="16"/>
-      <c r="G86" s="113"/>
+      <c r="G86" s="71"/>
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A87" s="71"/>
+      <c r="A87" s="85"/>
       <c r="B87" s="50" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="4"/>
       <c r="F87" s="16"/>
-      <c r="G87" s="113"/>
+      <c r="G87" s="71"/>
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A88" s="71"/>
+      <c r="A88" s="85"/>
       <c r="B88" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="4"/>
       <c r="F88" s="16"/>
-      <c r="G88" s="113"/>
-    </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A89" s="71"/>
-      <c r="B89" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="114"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="88">
+      <c r="G88" s="72"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="84">
         <v>10</v>
       </c>
-      <c r="B90" s="46" t="s">
+      <c r="B89" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C90" s="47"/>
-      <c r="D90" s="47"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="115"/>
+      <c r="C89" s="47"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="73"/>
+    </row>
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A90" s="84"/>
+      <c r="B90" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="74"/>
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="88"/>
-      <c r="B91" s="100" t="s">
-        <v>37</v>
-      </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
+      <c r="A91" s="84"/>
+      <c r="B91" s="81"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
       <c r="E91" s="4"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="116"/>
+      <c r="G91" s="74"/>
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A92" s="88"/>
-      <c r="B92" s="102"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+      <c r="A92" s="84"/>
+      <c r="B92" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
       <c r="E92" s="4"/>
       <c r="F92" s="16"/>
-      <c r="G92" s="116"/>
+      <c r="G92" s="74"/>
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A93" s="88"/>
+      <c r="A93" s="84"/>
       <c r="B93" s="50" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="4"/>
       <c r="F93" s="16"/>
-      <c r="G93" s="116"/>
+      <c r="G93" s="74"/>
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A94" s="88"/>
+      <c r="A94" s="84"/>
       <c r="B94" s="50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="4"/>
       <c r="F94" s="16"/>
-      <c r="G94" s="116"/>
-    </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A95" s="88"/>
-      <c r="B95" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="117"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="72">
+      <c r="G94" s="75"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="76">
         <v>11</v>
       </c>
-      <c r="B96" s="21" t="s">
+      <c r="B95" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C96" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="22"/>
-      <c r="E96" s="23"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="72"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="76"/>
+    </row>
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A96" s="77"/>
+      <c r="B96" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96" s="52"/>
+      <c r="D96" s="52"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="77"/>
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A97" s="73"/>
-      <c r="B97" s="101" t="s">
-        <v>37</v>
-      </c>
+      <c r="A97" s="77"/>
+      <c r="B97" s="83"/>
       <c r="C97" s="52"/>
       <c r="D97" s="52"/>
       <c r="E97" s="4"/>
       <c r="F97" s="16"/>
-      <c r="G97" s="73"/>
+      <c r="G97" s="77"/>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A98" s="73"/>
-      <c r="B98" s="101"/>
+      <c r="A98" s="77"/>
+      <c r="B98" s="83"/>
       <c r="C98" s="52"/>
       <c r="D98" s="52"/>
       <c r="E98" s="4"/>
       <c r="F98" s="16"/>
-      <c r="G98" s="73"/>
+      <c r="G98" s="77"/>
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A99" s="73"/>
-      <c r="B99" s="101"/>
+      <c r="A99" s="77"/>
+      <c r="B99" s="83"/>
       <c r="C99" s="52"/>
       <c r="D99" s="52"/>
       <c r="E99" s="4"/>
       <c r="F99" s="16"/>
-      <c r="G99" s="73"/>
+      <c r="G99" s="77"/>
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A100" s="73"/>
-      <c r="B100" s="101"/>
+      <c r="A100" s="77"/>
+      <c r="B100" s="83"/>
       <c r="C100" s="52"/>
       <c r="D100" s="52"/>
       <c r="E100" s="4"/>
       <c r="F100" s="16"/>
-      <c r="G100" s="73"/>
+      <c r="G100" s="77"/>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A101" s="73"/>
-      <c r="B101" s="101"/>
+      <c r="A101" s="77"/>
+      <c r="B101" s="83"/>
       <c r="C101" s="52"/>
       <c r="D101" s="52"/>
       <c r="E101" s="4"/>
       <c r="F101" s="16"/>
-      <c r="G101" s="73"/>
+      <c r="G101" s="77"/>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A102" s="73"/>
-      <c r="B102" s="101"/>
+      <c r="A102" s="77"/>
+      <c r="B102" s="83"/>
       <c r="C102" s="52"/>
       <c r="D102" s="52"/>
       <c r="E102" s="4"/>
       <c r="F102" s="16"/>
-      <c r="G102" s="73"/>
+      <c r="G102" s="77"/>
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A103" s="73"/>
-      <c r="B103" s="101"/>
-      <c r="C103" s="52"/>
-      <c r="D103" s="52"/>
+      <c r="A103" s="77"/>
+      <c r="B103" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
       <c r="E103" s="4"/>
       <c r="F103" s="16"/>
-      <c r="G103" s="73"/>
+      <c r="G103" s="77"/>
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A104" s="73"/>
+      <c r="A104" s="77"/>
       <c r="B104" s="53" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="4"/>
       <c r="F104" s="16"/>
-      <c r="G104" s="73"/>
+      <c r="G104" s="77"/>
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A105" s="73"/>
+      <c r="A105" s="78"/>
       <c r="B105" s="53" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="4"/>
       <c r="F105" s="16"/>
-      <c r="G105" s="73"/>
-    </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A106" s="74"/>
-      <c r="B106" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="16"/>
-      <c r="G106" s="74"/>
+      <c r="G105" s="78"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:F6" xr:uid="{60BF8AA0-547A-4AC4-BE58-D9F0611612D0}"/>
   <mergeCells count="44">
-    <mergeCell ref="G83:G89"/>
-    <mergeCell ref="G90:G95"/>
-    <mergeCell ref="G96:G106"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A77:A82"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A96:A106"/>
-    <mergeCell ref="B97:B103"/>
-    <mergeCell ref="A90:A95"/>
-    <mergeCell ref="A83:A89"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="A71:A76"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="G76:G81"/>
+    <mergeCell ref="G70:G75"/>
+    <mergeCell ref="G23:G32"/>
+    <mergeCell ref="G58:G63"/>
+    <mergeCell ref="G64:G69"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="D24:D32"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="G33:G41"/>
+    <mergeCell ref="G42:G49"/>
+    <mergeCell ref="G50:G57"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A22"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="A34:A42"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A41"/>
     <mergeCell ref="B13:B20"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="B24:B31"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B24:B30"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="D13:D22"/>
     <mergeCell ref="B2:G5"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="G77:G82"/>
-    <mergeCell ref="G71:G76"/>
-    <mergeCell ref="G23:G33"/>
-    <mergeCell ref="G59:G64"/>
-    <mergeCell ref="G65:G70"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="D24:D33"/>
-    <mergeCell ref="D35:D42"/>
     <mergeCell ref="G7:G11"/>
     <mergeCell ref="G12:G22"/>
-    <mergeCell ref="G34:G42"/>
-    <mergeCell ref="G43:G50"/>
-    <mergeCell ref="G51:G58"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="A76:A81"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="A95:A105"/>
+    <mergeCell ref="B96:B102"/>
+    <mergeCell ref="A89:A94"/>
+    <mergeCell ref="A82:A88"/>
+    <mergeCell ref="G82:G88"/>
+    <mergeCell ref="G89:G94"/>
+    <mergeCell ref="G95:G105"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B90:B91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Avanzamento Sprint3. Analisi dei Requisiti e del Problema.
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
+++ b/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\LORI\UNIVERSITA'\Magistrale\2°Anno\II Ciclo\Ingegneria dei Sistemi Software\Waiter_Robot\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2CF017-57EC-415A-9C2C-8A76D81C18BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED150643-CA24-4753-8813-096C5ADEB0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
   </bookViews>
@@ -730,95 +730,122 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -847,67 +874,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1993,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6357E3-4FBB-418C-9BB3-004C68F042FF}">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2011,51 +2011,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="102"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
     </row>
     <row r="3" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A3" s="69"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
     </row>
     <row r="4" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A4" s="69"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="114"/>
     </row>
     <row r="5" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A5" s="69"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="108"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="117"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
@@ -2079,7 +2079,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="100" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -2091,13 +2091,13 @@
       <c r="D7" s="54"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="100" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="92"/>
-      <c r="B8" s="94"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
@@ -2108,11 +2108,11 @@
       <c r="F8" s="11">
         <v>44002</v>
       </c>
-      <c r="G8" s="92"/>
+      <c r="G8" s="100"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
-      <c r="B9" s="95"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2123,11 +2123,11 @@
       <c r="F9" s="11">
         <v>44003</v>
       </c>
-      <c r="G9" s="92"/>
+      <c r="G9" s="100"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="92"/>
-      <c r="B10" s="95"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2138,11 +2138,11 @@
       <c r="F10" s="11">
         <v>44004</v>
       </c>
-      <c r="G10" s="92"/>
+      <c r="G10" s="100"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="92"/>
-      <c r="B11" s="96"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="108"/>
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
@@ -2153,10 +2153,10 @@
       <c r="F11" s="65">
         <v>44005</v>
       </c>
-      <c r="G11" s="92"/>
+      <c r="G11" s="100"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="85">
+      <c r="A12" s="101">
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -2168,162 +2168,162 @@
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="85" t="s">
+      <c r="G12" s="101" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85"/>
-      <c r="B13" s="80" t="s">
+      <c r="A13" s="101"/>
+      <c r="B13" s="103" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="97"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="11">
         <v>44006</v>
       </c>
-      <c r="G13" s="85"/>
+      <c r="G13" s="101"/>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="85"/>
-      <c r="B14" s="83"/>
+      <c r="A14" s="101"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="98"/>
+      <c r="D14" s="85"/>
       <c r="E14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="11">
         <v>44007</v>
       </c>
-      <c r="G14" s="85"/>
+      <c r="G14" s="101"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="85"/>
-      <c r="B15" s="83"/>
+      <c r="A15" s="101"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="98"/>
+      <c r="D15" s="85"/>
       <c r="E15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="11">
         <v>44007</v>
       </c>
-      <c r="G15" s="85"/>
+      <c r="G15" s="101"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="85"/>
-      <c r="B16" s="83"/>
+      <c r="A16" s="101"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="98"/>
+      <c r="D16" s="85"/>
       <c r="E16" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="85"/>
+      <c r="G16" s="101"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="85"/>
-      <c r="B17" s="83"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="98"/>
+      <c r="D17" s="85"/>
       <c r="E17" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="11">
         <v>44009</v>
       </c>
-      <c r="G17" s="85"/>
+      <c r="G17" s="101"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="85"/>
-      <c r="B18" s="83"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="98"/>
+      <c r="D18" s="85"/>
       <c r="E18" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="11">
         <v>44009</v>
       </c>
-      <c r="G18" s="85"/>
+      <c r="G18" s="101"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="85"/>
-      <c r="B19" s="83"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="98"/>
+      <c r="D19" s="85"/>
       <c r="E19" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="11">
         <v>44009</v>
       </c>
-      <c r="G19" s="85"/>
+      <c r="G19" s="101"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="85"/>
-      <c r="B20" s="81"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="98"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="11">
         <v>44009</v>
       </c>
-      <c r="G20" s="85"/>
+      <c r="G20" s="101"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="85"/>
+      <c r="A21" s="101"/>
       <c r="B21" s="50" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="98"/>
+      <c r="D21" s="85"/>
       <c r="E21" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="16">
         <v>44016</v>
       </c>
-      <c r="G21" s="85"/>
+      <c r="G21" s="101"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="85"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="99"/>
+      <c r="D22" s="86"/>
       <c r="E22" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="16">
         <v>44016</v>
       </c>
-      <c r="G22" s="85"/>
+      <c r="G22" s="101"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="84">
+      <c r="A23" s="77">
         <v>2</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -2335,147 +2335,147 @@
       <c r="D23" s="55"/>
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
-      <c r="G23" s="84" t="s">
+      <c r="G23" s="77" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
-      <c r="B24" s="80" t="s">
+      <c r="A24" s="77"/>
+      <c r="B24" s="103" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="97"/>
+      <c r="D24" s="84"/>
       <c r="E24" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="16">
         <v>44010</v>
       </c>
-      <c r="G24" s="84"/>
+      <c r="G24" s="77"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
-      <c r="B25" s="83"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="98"/>
+      <c r="D25" s="85"/>
       <c r="E25" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="16">
         <v>44012</v>
       </c>
-      <c r="G25" s="84"/>
+      <c r="G25" s="77"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
-      <c r="B26" s="83"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="98"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="16">
         <v>44012</v>
       </c>
-      <c r="G26" s="84"/>
+      <c r="G26" s="77"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="83"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="98"/>
+      <c r="D27" s="85"/>
       <c r="E27" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="16"/>
-      <c r="G27" s="84"/>
+      <c r="G27" s="77"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
-      <c r="B28" s="83"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="98"/>
+      <c r="D28" s="85"/>
       <c r="E28" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="16">
         <v>44013</v>
       </c>
-      <c r="G28" s="84"/>
+      <c r="G28" s="77"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
-      <c r="B29" s="83"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="98"/>
+      <c r="D29" s="85"/>
       <c r="E29" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="16">
         <v>44015</v>
       </c>
-      <c r="G29" s="84"/>
+      <c r="G29" s="77"/>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
-      <c r="B30" s="83"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="98"/>
+      <c r="D30" s="85"/>
       <c r="E30" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="16">
         <v>44016</v>
       </c>
-      <c r="G30" s="84"/>
+      <c r="G30" s="77"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="77"/>
       <c r="B31" s="60" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="98"/>
+      <c r="D31" s="85"/>
       <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F31" s="16">
         <v>44016</v>
       </c>
-      <c r="G31" s="84"/>
+      <c r="G31" s="77"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="99"/>
+      <c r="D32" s="86"/>
       <c r="E32" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="16">
         <v>44016</v>
       </c>
-      <c r="G32" s="84"/>
+      <c r="G32" s="77"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="93">
+      <c r="A33" s="102">
         <v>3</v>
       </c>
       <c r="B33" s="21" t="s">
@@ -2487,102 +2487,106 @@
       <c r="D33" s="22"/>
       <c r="E33" s="23"/>
       <c r="F33" s="24"/>
-      <c r="G33" s="76"/>
+      <c r="G33" s="90"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="93"/>
-      <c r="B34" s="80" t="s">
+      <c r="A34" s="102"/>
+      <c r="B34" s="103" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="121" t="s">
+      <c r="D34" s="87" t="s">
         <v>61</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="77"/>
+      <c r="F34" s="16">
+        <v>44017</v>
+      </c>
+      <c r="G34" s="91"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="93"/>
-      <c r="B35" s="83"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="122"/>
+      <c r="D35" s="88"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="77"/>
+      <c r="F35" s="16">
+        <v>44018</v>
+      </c>
+      <c r="G35" s="91"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="93"/>
-      <c r="B36" s="83"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="122"/>
+      <c r="D36" s="88"/>
       <c r="E36" s="4"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="77"/>
+      <c r="G36" s="91"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="93"/>
-      <c r="B37" s="83"/>
+      <c r="A37" s="102"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="122"/>
+      <c r="D37" s="88"/>
       <c r="E37" s="4"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="77"/>
+      <c r="G37" s="91"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="93"/>
-      <c r="B38" s="83"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="122"/>
+      <c r="D38" s="88"/>
       <c r="E38" s="4"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="77"/>
+      <c r="G38" s="91"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="93"/>
-      <c r="B39" s="81"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="122"/>
+      <c r="D39" s="88"/>
       <c r="E39" s="4"/>
       <c r="F39" s="16">
         <v>44018</v>
       </c>
-      <c r="G39" s="77"/>
+      <c r="G39" s="91"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="93"/>
+      <c r="A40" s="102"/>
       <c r="B40" s="50" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="64"/>
-      <c r="D40" s="122"/>
+      <c r="D40" s="88"/>
       <c r="E40" s="4"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="77"/>
+      <c r="G40" s="91"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="93"/>
+      <c r="A41" s="102"/>
       <c r="B41" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="123"/>
+      <c r="D41" s="89"/>
       <c r="E41" s="4"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="78"/>
+      <c r="G41" s="92"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="86">
+      <c r="A42" s="118">
         <v>4</v>
       </c>
       <c r="B42" s="25" t="s">
@@ -2594,59 +2598,59 @@
       <c r="D42" s="26"/>
       <c r="E42" s="27"/>
       <c r="F42" s="28"/>
-      <c r="G42" s="124"/>
+      <c r="G42" s="93"/>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="86"/>
-      <c r="B43" s="79" t="s">
+      <c r="A43" s="118"/>
+      <c r="B43" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="4"/>
       <c r="F43" s="16"/>
-      <c r="G43" s="125"/>
+      <c r="G43" s="94"/>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="86"/>
-      <c r="B44" s="79"/>
+      <c r="A44" s="118"/>
+      <c r="B44" s="70"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="4"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="125"/>
+      <c r="G44" s="94"/>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="86"/>
-      <c r="B45" s="79"/>
+      <c r="A45" s="118"/>
+      <c r="B45" s="70"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="4"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="125"/>
+      <c r="G45" s="94"/>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="86"/>
-      <c r="B46" s="79"/>
+      <c r="A46" s="118"/>
+      <c r="B46" s="70"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="4"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="125"/>
+      <c r="G46" s="94"/>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="86"/>
-      <c r="B47" s="79"/>
+      <c r="A47" s="118"/>
+      <c r="B47" s="70"/>
       <c r="C47" s="61"/>
       <c r="D47" s="61"/>
       <c r="E47" s="4"/>
       <c r="F47" s="16">
         <v>44022</v>
       </c>
-      <c r="G47" s="125"/>
+      <c r="G47" s="94"/>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="86"/>
+      <c r="A48" s="118"/>
       <c r="B48" s="50" t="s">
         <v>38</v>
       </c>
@@ -2654,10 +2658,10 @@
       <c r="D48" s="2"/>
       <c r="E48" s="4"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="125"/>
+      <c r="G48" s="94"/>
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="86"/>
+      <c r="A49" s="118"/>
       <c r="B49" s="50" t="s">
         <v>8</v>
       </c>
@@ -2665,10 +2669,10 @@
       <c r="D49" s="2"/>
       <c r="E49" s="4"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="126"/>
+      <c r="G49" s="95"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="87">
+      <c r="A50" s="119">
         <v>5</v>
       </c>
       <c r="B50" s="29" t="s">
@@ -2680,11 +2684,11 @@
       <c r="D50" s="30"/>
       <c r="E50" s="31"/>
       <c r="F50" s="32"/>
-      <c r="G50" s="127"/>
+      <c r="G50" s="96"/>
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A51" s="87"/>
-      <c r="B51" s="79" t="s">
+      <c r="A51" s="119"/>
+      <c r="B51" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -2693,44 +2697,44 @@
       <c r="D51" s="2"/>
       <c r="E51" s="4"/>
       <c r="F51" s="16"/>
-      <c r="G51" s="128"/>
+      <c r="G51" s="97"/>
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="87"/>
-      <c r="B52" s="79"/>
+      <c r="A52" s="119"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="4"/>
       <c r="F52" s="16"/>
-      <c r="G52" s="128"/>
+      <c r="G52" s="97"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="87"/>
-      <c r="B53" s="79"/>
+      <c r="A53" s="119"/>
+      <c r="B53" s="70"/>
       <c r="C53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="4"/>
       <c r="F53" s="16"/>
-      <c r="G53" s="128"/>
+      <c r="G53" s="97"/>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="87"/>
-      <c r="B54" s="79"/>
+      <c r="A54" s="119"/>
+      <c r="B54" s="70"/>
       <c r="C54" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="4"/>
       <c r="F54" s="16"/>
-      <c r="G54" s="128"/>
+      <c r="G54" s="97"/>
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="87"/>
-      <c r="B55" s="79"/>
+      <c r="A55" s="119"/>
+      <c r="B55" s="70"/>
       <c r="C55" s="2" t="s">
         <v>24</v>
       </c>
@@ -2739,10 +2743,10 @@
       <c r="F55" s="16">
         <v>44026</v>
       </c>
-      <c r="G55" s="128"/>
+      <c r="G55" s="97"/>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="87"/>
+      <c r="A56" s="119"/>
       <c r="B56" s="50" t="s">
         <v>38</v>
       </c>
@@ -2750,10 +2754,10 @@
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
       <c r="F56" s="16"/>
-      <c r="G56" s="128"/>
+      <c r="G56" s="97"/>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="87"/>
+      <c r="A57" s="119"/>
       <c r="B57" s="50" t="s">
         <v>8</v>
       </c>
@@ -2761,10 +2765,10 @@
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="129"/>
+      <c r="G57" s="98"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="88">
+      <c r="A58" s="120">
         <v>6</v>
       </c>
       <c r="B58" s="48" t="s">
@@ -2776,39 +2780,39 @@
       <c r="D58" s="49"/>
       <c r="E58" s="33"/>
       <c r="F58" s="34"/>
-      <c r="G58" s="115"/>
+      <c r="G58" s="78"/>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="88"/>
-      <c r="B59" s="79" t="s">
+      <c r="A59" s="120"/>
+      <c r="B59" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="4"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="116"/>
+      <c r="G59" s="79"/>
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" s="88"/>
-      <c r="B60" s="79"/>
+      <c r="A60" s="120"/>
+      <c r="B60" s="70"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="4"/>
       <c r="F60" s="16"/>
-      <c r="G60" s="116"/>
+      <c r="G60" s="79"/>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" s="88"/>
-      <c r="B61" s="79"/>
+      <c r="A61" s="120"/>
+      <c r="B61" s="70"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="4"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="116"/>
+      <c r="G61" s="79"/>
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A62" s="88"/>
+      <c r="A62" s="120"/>
       <c r="B62" s="50" t="s">
         <v>38</v>
       </c>
@@ -2816,10 +2820,10 @@
       <c r="D62" s="2"/>
       <c r="E62" s="4"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="116"/>
+      <c r="G62" s="79"/>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="88"/>
+      <c r="A63" s="120"/>
       <c r="B63" s="50" t="s">
         <v>8</v>
       </c>
@@ -2827,10 +2831,10 @@
       <c r="D63" s="2"/>
       <c r="E63" s="4"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="117"/>
+      <c r="G63" s="80"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="89">
+      <c r="A64" s="121">
         <v>6</v>
       </c>
       <c r="B64" s="35" t="s">
@@ -2840,39 +2844,39 @@
       <c r="D64" s="36"/>
       <c r="E64" s="37"/>
       <c r="F64" s="37"/>
-      <c r="G64" s="118"/>
+      <c r="G64" s="81"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="89"/>
-      <c r="B65" s="79" t="s">
+      <c r="A65" s="121"/>
+      <c r="B65" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="4"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="119"/>
+      <c r="G65" s="82"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="89"/>
-      <c r="B66" s="79"/>
+      <c r="A66" s="121"/>
+      <c r="B66" s="70"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="4"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="119"/>
+      <c r="G66" s="82"/>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A67" s="89"/>
-      <c r="B67" s="79"/>
+      <c r="A67" s="121"/>
+      <c r="B67" s="70"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="4"/>
       <c r="F67" s="16"/>
-      <c r="G67" s="119"/>
+      <c r="G67" s="82"/>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A68" s="89"/>
+      <c r="A68" s="121"/>
       <c r="B68" s="50" t="s">
         <v>38</v>
       </c>
@@ -2880,10 +2884,10 @@
       <c r="D68" s="2"/>
       <c r="E68" s="4"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="119"/>
+      <c r="G68" s="82"/>
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="89"/>
+      <c r="A69" s="121"/>
       <c r="B69" s="50" t="s">
         <v>8</v>
       </c>
@@ -2891,10 +2895,10 @@
       <c r="D69" s="2"/>
       <c r="E69" s="4"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="120"/>
+      <c r="G69" s="83"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="90">
+      <c r="A70" s="122">
         <v>7</v>
       </c>
       <c r="B70" s="38" t="s">
@@ -2904,39 +2908,39 @@
       <c r="D70" s="39"/>
       <c r="E70" s="40"/>
       <c r="F70" s="41"/>
-      <c r="G70" s="112"/>
+      <c r="G70" s="74"/>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A71" s="90"/>
-      <c r="B71" s="79" t="s">
+      <c r="A71" s="122"/>
+      <c r="B71" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="4"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="113"/>
+      <c r="G71" s="75"/>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="90"/>
-      <c r="B72" s="79"/>
+      <c r="A72" s="122"/>
+      <c r="B72" s="70"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="4"/>
       <c r="F72" s="16"/>
-      <c r="G72" s="113"/>
+      <c r="G72" s="75"/>
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A73" s="90"/>
-      <c r="B73" s="79"/>
+      <c r="A73" s="122"/>
+      <c r="B73" s="70"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="4"/>
       <c r="F73" s="16"/>
-      <c r="G73" s="113"/>
+      <c r="G73" s="75"/>
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A74" s="90"/>
+      <c r="A74" s="122"/>
       <c r="B74" s="50" t="s">
         <v>38</v>
       </c>
@@ -2944,10 +2948,10 @@
       <c r="D74" s="2"/>
       <c r="E74" s="4"/>
       <c r="F74" s="16"/>
-      <c r="G74" s="113"/>
+      <c r="G74" s="75"/>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A75" s="90"/>
+      <c r="A75" s="122"/>
       <c r="B75" s="50" t="s">
         <v>8</v>
       </c>
@@ -2955,10 +2959,10 @@
       <c r="D75" s="2"/>
       <c r="E75" s="4"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="114"/>
+      <c r="G75" s="76"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="82">
+      <c r="A76" s="123">
         <v>8</v>
       </c>
       <c r="B76" s="42" t="s">
@@ -2968,30 +2972,30 @@
       <c r="D76" s="43"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
-      <c r="G76" s="109"/>
+      <c r="G76" s="71"/>
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A77" s="82"/>
-      <c r="B77" s="79" t="s">
+      <c r="A77" s="123"/>
+      <c r="B77" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="4"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="110"/>
+      <c r="G77" s="72"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A78" s="82"/>
-      <c r="B78" s="79"/>
+      <c r="A78" s="123"/>
+      <c r="B78" s="70"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="4"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="110"/>
+      <c r="G78" s="72"/>
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A79" s="82"/>
+      <c r="A79" s="123"/>
       <c r="B79" s="50" t="s">
         <v>7</v>
       </c>
@@ -2999,10 +3003,10 @@
       <c r="D79" s="2"/>
       <c r="E79" s="4"/>
       <c r="F79" s="16"/>
-      <c r="G79" s="110"/>
+      <c r="G79" s="72"/>
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A80" s="82"/>
+      <c r="A80" s="123"/>
       <c r="B80" s="50" t="s">
         <v>38</v>
       </c>
@@ -3010,10 +3014,10 @@
       <c r="D80" s="2"/>
       <c r="E80" s="4"/>
       <c r="F80" s="16"/>
-      <c r="G80" s="110"/>
+      <c r="G80" s="72"/>
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A81" s="82"/>
+      <c r="A81" s="123"/>
       <c r="B81" s="50" t="s">
         <v>8</v>
       </c>
@@ -3021,10 +3025,10 @@
       <c r="D81" s="2"/>
       <c r="E81" s="4"/>
       <c r="F81" s="16"/>
-      <c r="G81" s="111"/>
+      <c r="G81" s="73"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="85">
+      <c r="A82" s="101">
         <v>9</v>
       </c>
       <c r="B82" s="12" t="s">
@@ -3034,39 +3038,39 @@
       <c r="D82" s="13"/>
       <c r="E82" s="14"/>
       <c r="F82" s="15"/>
-      <c r="G82" s="70"/>
+      <c r="G82" s="124"/>
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A83" s="85"/>
-      <c r="B83" s="79" t="s">
+      <c r="A83" s="101"/>
+      <c r="B83" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="4"/>
       <c r="F83" s="16"/>
-      <c r="G83" s="71"/>
+      <c r="G83" s="125"/>
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A84" s="85"/>
-      <c r="B84" s="79"/>
+      <c r="A84" s="101"/>
+      <c r="B84" s="70"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="4"/>
       <c r="F84" s="16"/>
-      <c r="G84" s="71"/>
+      <c r="G84" s="125"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A85" s="85"/>
-      <c r="B85" s="79"/>
+      <c r="A85" s="101"/>
+      <c r="B85" s="70"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="4"/>
       <c r="F85" s="16"/>
-      <c r="G85" s="71"/>
+      <c r="G85" s="125"/>
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A86" s="85"/>
+      <c r="A86" s="101"/>
       <c r="B86" s="50" t="s">
         <v>7</v>
       </c>
@@ -3074,10 +3078,10 @@
       <c r="D86" s="2"/>
       <c r="E86" s="4"/>
       <c r="F86" s="16"/>
-      <c r="G86" s="71"/>
+      <c r="G86" s="125"/>
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A87" s="85"/>
+      <c r="A87" s="101"/>
       <c r="B87" s="50" t="s">
         <v>38</v>
       </c>
@@ -3085,10 +3089,10 @@
       <c r="D87" s="2"/>
       <c r="E87" s="4"/>
       <c r="F87" s="16"/>
-      <c r="G87" s="71"/>
+      <c r="G87" s="125"/>
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A88" s="85"/>
+      <c r="A88" s="101"/>
       <c r="B88" s="50" t="s">
         <v>8</v>
       </c>
@@ -3096,10 +3100,10 @@
       <c r="D88" s="2"/>
       <c r="E88" s="4"/>
       <c r="F88" s="16"/>
-      <c r="G88" s="72"/>
+      <c r="G88" s="126"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="84">
+      <c r="A89" s="77">
         <v>10</v>
       </c>
       <c r="B89" s="46" t="s">
@@ -3109,30 +3113,30 @@
       <c r="D89" s="47"/>
       <c r="E89" s="19"/>
       <c r="F89" s="20"/>
-      <c r="G89" s="73"/>
+      <c r="G89" s="127"/>
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A90" s="84"/>
-      <c r="B90" s="80" t="s">
+      <c r="A90" s="77"/>
+      <c r="B90" s="103" t="s">
         <v>36</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="4"/>
       <c r="F90" s="16"/>
-      <c r="G90" s="74"/>
+      <c r="G90" s="128"/>
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="84"/>
-      <c r="B91" s="81"/>
+      <c r="A91" s="77"/>
+      <c r="B91" s="105"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="4"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="74"/>
+      <c r="G91" s="128"/>
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A92" s="84"/>
+      <c r="A92" s="77"/>
       <c r="B92" s="50" t="s">
         <v>7</v>
       </c>
@@ -3140,10 +3144,10 @@
       <c r="D92" s="2"/>
       <c r="E92" s="4"/>
       <c r="F92" s="16"/>
-      <c r="G92" s="74"/>
+      <c r="G92" s="128"/>
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A93" s="84"/>
+      <c r="A93" s="77"/>
       <c r="B93" s="50" t="s">
         <v>38</v>
       </c>
@@ -3151,10 +3155,10 @@
       <c r="D93" s="2"/>
       <c r="E93" s="4"/>
       <c r="F93" s="16"/>
-      <c r="G93" s="74"/>
+      <c r="G93" s="128"/>
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A94" s="84"/>
+      <c r="A94" s="77"/>
       <c r="B94" s="50" t="s">
         <v>8</v>
       </c>
@@ -3162,10 +3166,10 @@
       <c r="D94" s="2"/>
       <c r="E94" s="4"/>
       <c r="F94" s="16"/>
-      <c r="G94" s="75"/>
+      <c r="G94" s="129"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="76">
+      <c r="A95" s="90">
         <v>11</v>
       </c>
       <c r="B95" s="21" t="s">
@@ -3175,75 +3179,75 @@
       <c r="D95" s="22"/>
       <c r="E95" s="23"/>
       <c r="F95" s="24"/>
-      <c r="G95" s="76"/>
+      <c r="G95" s="90"/>
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A96" s="77"/>
-      <c r="B96" s="83" t="s">
+      <c r="A96" s="91"/>
+      <c r="B96" s="104" t="s">
         <v>36</v>
       </c>
       <c r="C96" s="52"/>
       <c r="D96" s="52"/>
       <c r="E96" s="4"/>
       <c r="F96" s="16"/>
-      <c r="G96" s="77"/>
+      <c r="G96" s="91"/>
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A97" s="77"/>
-      <c r="B97" s="83"/>
+      <c r="A97" s="91"/>
+      <c r="B97" s="104"/>
       <c r="C97" s="52"/>
       <c r="D97" s="52"/>
       <c r="E97" s="4"/>
       <c r="F97" s="16"/>
-      <c r="G97" s="77"/>
+      <c r="G97" s="91"/>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A98" s="77"/>
-      <c r="B98" s="83"/>
+      <c r="A98" s="91"/>
+      <c r="B98" s="104"/>
       <c r="C98" s="52"/>
       <c r="D98" s="52"/>
       <c r="E98" s="4"/>
       <c r="F98" s="16"/>
-      <c r="G98" s="77"/>
+      <c r="G98" s="91"/>
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A99" s="77"/>
-      <c r="B99" s="83"/>
+      <c r="A99" s="91"/>
+      <c r="B99" s="104"/>
       <c r="C99" s="52"/>
       <c r="D99" s="52"/>
       <c r="E99" s="4"/>
       <c r="F99" s="16"/>
-      <c r="G99" s="77"/>
+      <c r="G99" s="91"/>
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A100" s="77"/>
-      <c r="B100" s="83"/>
+      <c r="A100" s="91"/>
+      <c r="B100" s="104"/>
       <c r="C100" s="52"/>
       <c r="D100" s="52"/>
       <c r="E100" s="4"/>
       <c r="F100" s="16"/>
-      <c r="G100" s="77"/>
+      <c r="G100" s="91"/>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A101" s="77"/>
-      <c r="B101" s="83"/>
+      <c r="A101" s="91"/>
+      <c r="B101" s="104"/>
       <c r="C101" s="52"/>
       <c r="D101" s="52"/>
       <c r="E101" s="4"/>
       <c r="F101" s="16"/>
-      <c r="G101" s="77"/>
+      <c r="G101" s="91"/>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A102" s="77"/>
-      <c r="B102" s="83"/>
+      <c r="A102" s="91"/>
+      <c r="B102" s="104"/>
       <c r="C102" s="52"/>
       <c r="D102" s="52"/>
       <c r="E102" s="4"/>
       <c r="F102" s="16"/>
-      <c r="G102" s="77"/>
+      <c r="G102" s="91"/>
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A103" s="77"/>
+      <c r="A103" s="91"/>
       <c r="B103" s="53" t="s">
         <v>7</v>
       </c>
@@ -3251,10 +3255,10 @@
       <c r="D103" s="2"/>
       <c r="E103" s="4"/>
       <c r="F103" s="16"/>
-      <c r="G103" s="77"/>
+      <c r="G103" s="91"/>
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A104" s="77"/>
+      <c r="A104" s="91"/>
       <c r="B104" s="53" t="s">
         <v>38</v>
       </c>
@@ -3262,10 +3266,10 @@
       <c r="D104" s="2"/>
       <c r="E104" s="4"/>
       <c r="F104" s="16"/>
-      <c r="G104" s="77"/>
+      <c r="G104" s="91"/>
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A105" s="78"/>
+      <c r="A105" s="92"/>
       <c r="B105" s="53" t="s">
         <v>8</v>
       </c>
@@ -3273,11 +3277,40 @@
       <c r="D105" s="2"/>
       <c r="E105" s="4"/>
       <c r="F105" s="16"/>
-      <c r="G105" s="78"/>
+      <c r="G105" s="92"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:F6" xr:uid="{60BF8AA0-547A-4AC4-BE58-D9F0611612D0}"/>
   <mergeCells count="44">
+    <mergeCell ref="G82:G88"/>
+    <mergeCell ref="G89:G94"/>
+    <mergeCell ref="G95:G105"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="A76:A81"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="A95:A105"/>
+    <mergeCell ref="B96:B102"/>
+    <mergeCell ref="A89:A94"/>
+    <mergeCell ref="A82:A88"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="D13:D22"/>
+    <mergeCell ref="B2:G5"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G12:G22"/>
     <mergeCell ref="B65:B67"/>
     <mergeCell ref="G76:G81"/>
     <mergeCell ref="G70:G75"/>
@@ -3293,35 +3326,6 @@
     <mergeCell ref="G33:G41"/>
     <mergeCell ref="G42:G49"/>
     <mergeCell ref="G50:G57"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="B13:B20"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="D13:D22"/>
-    <mergeCell ref="B2:G5"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G12:G22"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="A64:A69"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="A76:A81"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="A95:A105"/>
-    <mergeCell ref="B96:B102"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="A82:A88"/>
-    <mergeCell ref="G82:G88"/>
-    <mergeCell ref="G89:G94"/>
-    <mergeCell ref="G95:G105"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="B90:B91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Realizzata webGUI. Quasi ultimato Sprint3
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
+++ b/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\LORI\UNIVERSITA'\Magistrale\2°Anno\II Ciclo\Ingegneria dei Sistemi Software\Waiter_Robot\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED150643-CA24-4753-8813-096C5ADEB0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049FB4ED-6361-41AE-AFB0-1001E4BEC86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
+    <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
   <si>
     <t>Sprint Goal (obiettivo)</t>
   </si>
@@ -93,12 +93,6 @@
     <t>Realizzare una base di conoscenza.</t>
   </si>
   <si>
-    <t>4.1 Front-end</t>
-  </si>
-  <si>
-    <t>4.2 Back-end</t>
-  </si>
-  <si>
     <t>Redarre un'overview iniziale</t>
   </si>
   <si>
@@ -120,12 +114,6 @@
     <t>Creazione di una KB della room</t>
   </si>
   <si>
-    <t>Gestione "non ottimizzata" di più clienti</t>
-  </si>
-  <si>
-    <t>Ottimizzazione del waiter</t>
-  </si>
-  <si>
     <t>Analisi del Problema (+ revisione del modello eseguibile)</t>
   </si>
   <si>
@@ -220,11 +208,14 @@
   </si>
   <si>
     <t>Implementare il MaxStayTime Countdown</t>
+  </si>
+  <si>
+    <t>Gestione di più clienti</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">1) Si rilassa il vincolo de "un solo cliente in sala". Ora possono arrivare tutte le richieste di ingresso che si vuole.
-2) Al barman, di conseguenza, potrà essere richiesto di lavorare alla preparazione di più ordini, anche in parallelo. 
+2) Il barman non è in grado di lavorare in parallelo a più ordini. Le preparazioni, supposte di breve durata, sono sequenziali. 
 3) Il tempo di preparazione di un ordine è sempre lo stesso, a prescindere da cosa è stato ordinato.
 4) I task del waiter </t>
     </r>
@@ -249,6 +240,18 @@
       </rPr>
       <t xml:space="preserve"> sono interrompibili.</t>
     </r>
+  </si>
+  <si>
+    <t>Eventuali ottimizzazioni del waiter</t>
+  </si>
+  <si>
+    <t>Aggiornamento KB della tearoom</t>
+  </si>
+  <si>
+    <t>Client simulator</t>
+  </si>
+  <si>
+    <t>webGUI</t>
   </si>
 </sst>
 </file>
@@ -1210,13 +1213,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3840480</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1275,7 +1278,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="it-IT" sz="1100"/>
-            <a:t>2) Al barman, di conseguenza, potrà essere richiesto di lavorare alla preparazione di più ordini, anche in parallelo. </a:t>
+            <a:t>2) Il barman non è in grado di lavorare in parallelo a più ordini. Le preparazioni, supposte di breve durata, sono sequenziali. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1287,7 +1290,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="it-IT" sz="1100"/>
-            <a:t>4) I task del waiter non sono interrompibili.</a:t>
+            <a:t>4) I task del waiter </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1"/>
+            <a:t>non</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100"/>
+            <a:t> sono interrompibili.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1298,13 +1309,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3840480</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1816,7 +1827,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1845,16 +1856,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="68"/>
       <c r="B3" s="67" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1862,10 +1873,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1876,7 +1887,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1887,7 +1898,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1895,7 +1906,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1903,7 +1914,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1911,7 +1922,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1919,7 +1930,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1927,7 +1938,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1935,39 +1946,33 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="68">
         <v>11</v>
       </c>
-      <c r="B13" s="67" t="s">
-        <v>18</v>
+      <c r="B13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="68">
         <v>12</v>
       </c>
-      <c r="B14" s="67" t="s">
-        <v>19</v>
+      <c r="B14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="68">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="68">
         <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1991,10 +1996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6357E3-4FBB-418C-9BB3-004C68F042FF}">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2012,7 +2017,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -2068,7 +2073,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>4</v>
@@ -2083,10 +2088,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="54"/>
       <c r="E7" s="9"/>
@@ -2099,7 +2104,7 @@
       <c r="A8" s="100"/>
       <c r="B8" s="106"/>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
@@ -2114,7 +2119,7 @@
       <c r="A9" s="100"/>
       <c r="B9" s="107"/>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
@@ -2129,7 +2134,7 @@
       <c r="A10" s="100"/>
       <c r="B10" s="107"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="s">
@@ -2144,7 +2149,7 @@
       <c r="A11" s="100"/>
       <c r="B11" s="108"/>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
@@ -2160,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
@@ -2175,10 +2180,10 @@
     <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="101"/>
       <c r="B13" s="103" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="84"/>
       <c r="E13" s="4" t="s">
@@ -2193,7 +2198,7 @@
       <c r="A14" s="101"/>
       <c r="B14" s="104"/>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D14" s="85"/>
       <c r="E14" s="4" t="s">
@@ -2223,7 +2228,7 @@
       <c r="A16" s="101"/>
       <c r="B16" s="104"/>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="85"/>
       <c r="E16" s="4" t="s">
@@ -2236,7 +2241,7 @@
       <c r="A17" s="101"/>
       <c r="B17" s="104"/>
       <c r="C17" s="64" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17" s="85"/>
       <c r="E17" s="4" t="s">
@@ -2251,7 +2256,7 @@
       <c r="A18" s="101"/>
       <c r="B18" s="104"/>
       <c r="C18" s="66" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D18" s="85"/>
       <c r="E18" s="4" t="s">
@@ -2266,7 +2271,7 @@
       <c r="A19" s="101"/>
       <c r="B19" s="104"/>
       <c r="C19" s="62" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D19" s="85"/>
       <c r="E19" s="4" t="s">
@@ -2281,7 +2286,7 @@
       <c r="A20" s="101"/>
       <c r="B20" s="105"/>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" s="85"/>
       <c r="E20" s="4" t="s">
@@ -2295,7 +2300,7 @@
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="101"/>
       <c r="B21" s="50" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="85"/>
@@ -2327,10 +2332,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" s="55"/>
       <c r="E23" s="19"/>
@@ -2342,10 +2347,10 @@
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="77"/>
       <c r="B24" s="103" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D24" s="84"/>
       <c r="E24" s="4" t="s">
@@ -2360,7 +2365,7 @@
       <c r="A25" s="77"/>
       <c r="B25" s="104"/>
       <c r="C25" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D25" s="85"/>
       <c r="E25" s="4" t="s">
@@ -2390,7 +2395,7 @@
       <c r="A27" s="77"/>
       <c r="B27" s="104"/>
       <c r="C27" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" s="85"/>
       <c r="E27" s="4" t="s">
@@ -2403,7 +2408,7 @@
       <c r="A28" s="77"/>
       <c r="B28" s="104"/>
       <c r="C28" s="63" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="85"/>
       <c r="E28" s="4" t="s">
@@ -2418,7 +2423,7 @@
       <c r="A29" s="77"/>
       <c r="B29" s="104"/>
       <c r="C29" s="63" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D29" s="85"/>
       <c r="E29" s="4" t="s">
@@ -2433,7 +2438,7 @@
       <c r="A30" s="77"/>
       <c r="B30" s="104"/>
       <c r="C30" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D30" s="85"/>
       <c r="E30" s="4" t="s">
@@ -2447,7 +2452,7 @@
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="77"/>
       <c r="B31" s="60" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="85"/>
@@ -2479,10 +2484,10 @@
         <v>3</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="23"/>
@@ -2492,13 +2497,13 @@
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="102"/>
       <c r="B34" s="103" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D34" s="87" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="16">
@@ -2510,7 +2515,7 @@
       <c r="A35" s="102"/>
       <c r="B35" s="104"/>
       <c r="C35" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D35" s="88"/>
       <c r="E35" s="4"/>
@@ -2527,14 +2532,16 @@
       </c>
       <c r="D36" s="88"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="16"/>
+      <c r="F36" s="16">
+        <v>44020</v>
+      </c>
       <c r="G36" s="91"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" s="102"/>
       <c r="B37" s="104"/>
       <c r="C37" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D37" s="88"/>
       <c r="E37" s="4"/>
@@ -2544,85 +2551,97 @@
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="102"/>
       <c r="B38" s="104"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="62" t="s">
+        <v>60</v>
+      </c>
       <c r="D38" s="88"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="16"/>
+      <c r="F38" s="16">
+        <v>44022</v>
+      </c>
       <c r="G38" s="91"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="102"/>
-      <c r="B39" s="105"/>
-      <c r="C39" s="2" t="s">
-        <v>24</v>
+      <c r="B39" s="104"/>
+      <c r="C39" s="62" t="s">
+        <v>61</v>
       </c>
       <c r="D39" s="88"/>
       <c r="E39" s="4"/>
       <c r="F39" s="16">
-        <v>44018</v>
+        <v>44022</v>
       </c>
       <c r="G39" s="91"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="102"/>
-      <c r="B40" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="64"/>
+      <c r="B40" s="104"/>
+      <c r="C40" s="62" t="s">
+        <v>62</v>
+      </c>
       <c r="D40" s="88"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="16"/>
+      <c r="F40" s="16">
+        <v>44022</v>
+      </c>
       <c r="G40" s="91"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" s="102"/>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="105"/>
+      <c r="C41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="88"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="16">
+        <v>44023</v>
+      </c>
+      <c r="G41" s="91"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A42" s="102"/>
+      <c r="B42" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="64"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="91"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A43" s="102"/>
+      <c r="B43" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="92"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="118">
-        <v>4</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="93"/>
-    </row>
-    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="118"/>
-      <c r="B43" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="89"/>
       <c r="E43" s="4"/>
       <c r="F43" s="16"/>
-      <c r="G43" s="94"/>
-    </row>
-    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="118"/>
-      <c r="B44" s="70"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="94"/>
+      <c r="G43" s="92"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="118">
+        <v>4</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="93"/>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" s="118"/>
-      <c r="B45" s="70"/>
+      <c r="B45" s="70" t="s">
+        <v>32</v>
+      </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="4"/>
@@ -2641,19 +2660,15 @@
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" s="118"/>
       <c r="B47" s="70"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
       <c r="E47" s="4"/>
-      <c r="F47" s="16">
-        <v>44022</v>
-      </c>
+      <c r="F47" s="16"/>
       <c r="G47" s="94"/>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A48" s="118"/>
-      <c r="B48" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="B48" s="70"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="4"/>
@@ -2662,59 +2677,59 @@
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A49" s="118"/>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="70"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="16">
+        <v>44022</v>
+      </c>
+      <c r="G49" s="94"/>
+    </row>
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A50" s="118"/>
+      <c r="B50" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="94"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A51" s="118"/>
+      <c r="B51" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="95"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="119">
-        <v>5</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" s="30"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="96"/>
-    </row>
-    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A51" s="119"/>
-      <c r="B51" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="4"/>
       <c r="F51" s="16"/>
-      <c r="G51" s="97"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="119"/>
-      <c r="B52" s="70"/>
-      <c r="C52" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="97"/>
+      <c r="G51" s="95"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="119">
+        <v>5</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="30"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="96"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A53" s="119"/>
-      <c r="B53" s="70"/>
+      <c r="B53" s="70" t="s">
+        <v>32</v>
+      </c>
       <c r="C53" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="4"/>
@@ -2724,7 +2739,7 @@
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A54" s="119"/>
       <c r="B54" s="70"/>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="2"/>
@@ -2736,21 +2751,19 @@
       <c r="A55" s="119"/>
       <c r="B55" s="70"/>
       <c r="C55" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="16">
-        <v>44026</v>
-      </c>
+      <c r="F55" s="16"/>
       <c r="G55" s="97"/>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A56" s="119"/>
-      <c r="B56" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="5"/>
+      <c r="B56" s="70"/>
+      <c r="C56" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
       <c r="F56" s="16"/>
@@ -2758,53 +2771,59 @@
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A57" s="119"/>
-      <c r="B57" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="5"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="98"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="120">
-        <v>6</v>
-      </c>
-      <c r="B58" s="48" t="s">
+      <c r="F57" s="16">
+        <v>44026</v>
+      </c>
+      <c r="G57" s="97"/>
+    </row>
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A58" s="119"/>
+      <c r="B58" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="D58" s="49"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="78"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="97"/>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="120"/>
-      <c r="B59" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="2"/>
+      <c r="A59" s="119"/>
+      <c r="B59" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="5"/>
       <c r="D59" s="2"/>
       <c r="E59" s="4"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="79"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" s="120"/>
-      <c r="B60" s="70"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="79"/>
+      <c r="G59" s="98"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="120">
+        <v>6</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="49"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="78"/>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A61" s="120"/>
-      <c r="B61" s="70"/>
+      <c r="B61" s="70" t="s">
+        <v>32</v>
+      </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="4"/>
@@ -2813,9 +2832,7 @@
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A62" s="120"/>
-      <c r="B62" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="B62" s="70"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="4"/>
@@ -2824,51 +2841,53 @@
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A63" s="120"/>
-      <c r="B63" s="50" t="s">
-        <v>8</v>
-      </c>
+      <c r="B63" s="70"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="4"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="80"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="121">
-        <v>6</v>
-      </c>
-      <c r="B64" s="35" t="s">
+      <c r="G63" s="79"/>
+    </row>
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A64" s="120"/>
+      <c r="B64" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="81"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="79"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="121"/>
-      <c r="B65" s="70" t="s">
-        <v>36</v>
+      <c r="A65" s="120"/>
+      <c r="B65" s="50" t="s">
+        <v>8</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="4"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="82"/>
-    </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="121"/>
-      <c r="B66" s="70"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="82"/>
+      <c r="G65" s="80"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="121">
+        <v>6</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="81"/>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="121"/>
-      <c r="B67" s="70"/>
+      <c r="B67" s="70" t="s">
+        <v>32</v>
+      </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="4"/>
@@ -2877,9 +2896,7 @@
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A68" s="121"/>
-      <c r="B68" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="B68" s="70"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="4"/>
@@ -2888,51 +2905,53 @@
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A69" s="121"/>
-      <c r="B69" s="50" t="s">
-        <v>8</v>
-      </c>
+      <c r="B69" s="70"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="4"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="83"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="122">
-        <v>7</v>
-      </c>
-      <c r="B70" s="38" t="s">
+      <c r="G69" s="82"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A70" s="121"/>
+      <c r="B70" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="41"/>
-      <c r="G70" s="74"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="82"/>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A71" s="122"/>
-      <c r="B71" s="70" t="s">
-        <v>36</v>
+      <c r="A71" s="121"/>
+      <c r="B71" s="50" t="s">
+        <v>8</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="4"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="75"/>
-    </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="122"/>
-      <c r="B72" s="70"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="75"/>
+      <c r="G71" s="83"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="122">
+        <v>7</v>
+      </c>
+      <c r="B72" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="74"/>
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A73" s="122"/>
-      <c r="B73" s="70"/>
+      <c r="B73" s="70" t="s">
+        <v>32</v>
+      </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="4"/>
@@ -2941,9 +2960,7 @@
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A74" s="122"/>
-      <c r="B74" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="B74" s="70"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="4"/>
@@ -2952,52 +2969,52 @@
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A75" s="122"/>
-      <c r="B75" s="50" t="s">
-        <v>8</v>
-      </c>
+      <c r="B75" s="70"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="4"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="76"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="123">
+      <c r="G75" s="75"/>
+    </row>
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A76" s="122"/>
+      <c r="B76" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="75"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A77" s="122"/>
+      <c r="B77" s="50" t="s">
         <v>8</v>
-      </c>
-      <c r="B76" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C76" s="43"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="71"/>
-    </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A77" s="123"/>
-      <c r="B77" s="70" t="s">
-        <v>36</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="4"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="72"/>
-    </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A78" s="123"/>
-      <c r="B78" s="70"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="72"/>
+      <c r="G77" s="76"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="123">
+        <v>8</v>
+      </c>
+      <c r="B78" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="71"/>
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A79" s="123"/>
-      <c r="B79" s="50" t="s">
-        <v>7</v>
+      <c r="B79" s="70" t="s">
+        <v>32</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -3007,9 +3024,7 @@
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A80" s="123"/>
-      <c r="B80" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="B80" s="70"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="4"/>
@@ -3019,50 +3034,54 @@
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A81" s="123"/>
       <c r="B81" s="50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="4"/>
       <c r="F81" s="16"/>
-      <c r="G81" s="73"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="101">
-        <v>9</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="15"/>
-      <c r="G82" s="124"/>
+      <c r="G81" s="72"/>
+    </row>
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A82" s="123"/>
+      <c r="B82" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="72"/>
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A83" s="101"/>
-      <c r="B83" s="70" t="s">
-        <v>36</v>
+      <c r="A83" s="123"/>
+      <c r="B83" s="50" t="s">
+        <v>8</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="4"/>
       <c r="F83" s="16"/>
-      <c r="G83" s="125"/>
-    </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A84" s="101"/>
-      <c r="B84" s="70"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="125"/>
+      <c r="G83" s="73"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="101">
+        <v>9</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="124"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A85" s="101"/>
-      <c r="B85" s="70"/>
+      <c r="B85" s="70" t="s">
+        <v>32</v>
+      </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="4"/>
@@ -3071,9 +3090,7 @@
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A86" s="101"/>
-      <c r="B86" s="50" t="s">
-        <v>7</v>
-      </c>
+      <c r="B86" s="70"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="4"/>
@@ -3082,9 +3099,7 @@
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A87" s="101"/>
-      <c r="B87" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="B87" s="70"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="4"/>
@@ -3094,51 +3109,53 @@
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A88" s="101"/>
       <c r="B88" s="50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="4"/>
       <c r="F88" s="16"/>
-      <c r="G88" s="126"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="77">
-        <v>10</v>
-      </c>
-      <c r="B89" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C89" s="47"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="127"/>
+      <c r="G88" s="125"/>
+    </row>
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A89" s="101"/>
+      <c r="B89" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="125"/>
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A90" s="77"/>
-      <c r="B90" s="103" t="s">
-        <v>36</v>
+      <c r="A90" s="101"/>
+      <c r="B90" s="50" t="s">
+        <v>8</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="4"/>
       <c r="F90" s="16"/>
-      <c r="G90" s="128"/>
-    </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="77"/>
-      <c r="B91" s="105"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="128"/>
+      <c r="G90" s="126"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="77">
+        <v>10</v>
+      </c>
+      <c r="B91" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="47"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="127"/>
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A92" s="77"/>
-      <c r="B92" s="50" t="s">
-        <v>7</v>
+      <c r="B92" s="103" t="s">
+        <v>32</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -3148,11 +3165,9 @@
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A93" s="77"/>
-      <c r="B93" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
+      <c r="B93" s="105"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
       <c r="E93" s="4"/>
       <c r="F93" s="16"/>
       <c r="G93" s="128"/>
@@ -3160,50 +3175,54 @@
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A94" s="77"/>
       <c r="B94" s="50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="4"/>
       <c r="F94" s="16"/>
-      <c r="G94" s="129"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="90">
-        <v>11</v>
-      </c>
-      <c r="B95" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C95" s="22"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="23"/>
-      <c r="F95" s="24"/>
-      <c r="G95" s="90"/>
+      <c r="G94" s="128"/>
+    </row>
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A95" s="77"/>
+      <c r="B95" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="128"/>
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A96" s="91"/>
-      <c r="B96" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="C96" s="52"/>
-      <c r="D96" s="52"/>
+      <c r="A96" s="77"/>
+      <c r="B96" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
       <c r="E96" s="4"/>
       <c r="F96" s="16"/>
-      <c r="G96" s="91"/>
-    </row>
-    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A97" s="91"/>
-      <c r="B97" s="104"/>
-      <c r="C97" s="52"/>
-      <c r="D97" s="52"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="91"/>
+      <c r="G96" s="129"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" s="90">
+        <v>11</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="90"/>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A98" s="91"/>
-      <c r="B98" s="104"/>
+      <c r="B98" s="104" t="s">
+        <v>32</v>
+      </c>
       <c r="C98" s="52"/>
       <c r="D98" s="52"/>
       <c r="E98" s="4"/>
@@ -3248,84 +3267,102 @@
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A103" s="91"/>
-      <c r="B103" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
+      <c r="B103" s="104"/>
+      <c r="C103" s="52"/>
+      <c r="D103" s="52"/>
       <c r="E103" s="4"/>
       <c r="F103" s="16"/>
       <c r="G103" s="91"/>
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A104" s="91"/>
-      <c r="B104" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
+      <c r="B104" s="104"/>
+      <c r="C104" s="52"/>
+      <c r="D104" s="52"/>
       <c r="E104" s="4"/>
       <c r="F104" s="16"/>
       <c r="G104" s="91"/>
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A105" s="92"/>
+      <c r="A105" s="91"/>
       <c r="B105" s="53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="4"/>
       <c r="F105" s="16"/>
-      <c r="G105" s="92"/>
+      <c r="G105" s="91"/>
+    </row>
+    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A106" s="91"/>
+      <c r="B106" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="91"/>
+    </row>
+    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A107" s="92"/>
+      <c r="B107" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="92"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:F6" xr:uid="{60BF8AA0-547A-4AC4-BE58-D9F0611612D0}"/>
   <mergeCells count="44">
-    <mergeCell ref="G82:G88"/>
-    <mergeCell ref="G89:G94"/>
-    <mergeCell ref="G95:G105"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="A76:A81"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="A95:A105"/>
-    <mergeCell ref="B96:B102"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="A82:A88"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="A64:A69"/>
-    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="G84:G90"/>
+    <mergeCell ref="G91:G96"/>
+    <mergeCell ref="G97:G107"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A78:A83"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="A97:A107"/>
+    <mergeCell ref="B98:B104"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A84:A90"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="A66:A71"/>
+    <mergeCell ref="A72:A77"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A22"/>
     <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A33:A43"/>
     <mergeCell ref="B13:B20"/>
-    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B34:B41"/>
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="D13:D22"/>
     <mergeCell ref="B2:G5"/>
     <mergeCell ref="G7:G11"/>
     <mergeCell ref="G12:G22"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="G76:G81"/>
-    <mergeCell ref="G70:G75"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="G78:G83"/>
+    <mergeCell ref="G72:G77"/>
     <mergeCell ref="G23:G32"/>
-    <mergeCell ref="G58:G63"/>
-    <mergeCell ref="G64:G69"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="G60:G65"/>
+    <mergeCell ref="G66:G71"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B79:B80"/>
     <mergeCell ref="D24:D32"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="G33:G41"/>
-    <mergeCell ref="G42:G49"/>
-    <mergeCell ref="G50:G57"/>
+    <mergeCell ref="D34:D43"/>
+    <mergeCell ref="G33:G43"/>
+    <mergeCell ref="G44:G51"/>
+    <mergeCell ref="G52:G59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Testing Sprint4 + creato script esecuzione
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
+++ b/DOCUMENTS/Workplan+Assunzioni e Vincoli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\LORI\UNIVERSITA'\Magistrale\2°Anno\II Ciclo\Ingegneria dei Sistemi Software\Waiter_Robot\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF1B6E9-170A-45A2-8D76-BA879649EF84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25B6D87-28FE-4A3F-89C4-0406F2D14144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
   <si>
     <t>Sprint Goal (obiettivo)</t>
   </si>
@@ -739,95 +739,122 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -856,67 +883,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2004,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6357E3-4FBB-418C-9BB3-004C68F042FF}">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2022,51 +2022,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="102"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
     </row>
     <row r="3" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A3" s="69"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
     </row>
     <row r="4" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A4" s="69"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="114"/>
     </row>
     <row r="5" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A5" s="69"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="108"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="117"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
@@ -2090,7 +2090,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="100" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -2102,13 +2102,13 @@
       <c r="D7" s="54"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="100" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="92"/>
-      <c r="B8" s="94"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
@@ -2119,11 +2119,11 @@
       <c r="F8" s="11">
         <v>44002</v>
       </c>
-      <c r="G8" s="92"/>
+      <c r="G8" s="100"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
-      <c r="B9" s="95"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2134,11 +2134,11 @@
       <c r="F9" s="11">
         <v>44003</v>
       </c>
-      <c r="G9" s="92"/>
+      <c r="G9" s="100"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="92"/>
-      <c r="B10" s="95"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
@@ -2149,11 +2149,11 @@
       <c r="F10" s="11">
         <v>44004</v>
       </c>
-      <c r="G10" s="92"/>
+      <c r="G10" s="100"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="92"/>
-      <c r="B11" s="96"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="108"/>
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2164,10 +2164,10 @@
       <c r="F11" s="65">
         <v>44005</v>
       </c>
-      <c r="G11" s="92"/>
+      <c r="G11" s="100"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="85">
+      <c r="A12" s="101">
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -2179,162 +2179,162 @@
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="85" t="s">
+      <c r="G12" s="101" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85"/>
-      <c r="B13" s="80" t="s">
+      <c r="A13" s="101"/>
+      <c r="B13" s="103" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="97"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="11">
         <v>44006</v>
       </c>
-      <c r="G13" s="85"/>
+      <c r="G13" s="101"/>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="85"/>
-      <c r="B14" s="83"/>
+      <c r="A14" s="101"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="98"/>
+      <c r="D14" s="85"/>
       <c r="E14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="11">
         <v>44007</v>
       </c>
-      <c r="G14" s="85"/>
+      <c r="G14" s="101"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="85"/>
-      <c r="B15" s="83"/>
+      <c r="A15" s="101"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="98"/>
+      <c r="D15" s="85"/>
       <c r="E15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="11">
         <v>44007</v>
       </c>
-      <c r="G15" s="85"/>
+      <c r="G15" s="101"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="85"/>
-      <c r="B16" s="83"/>
+      <c r="A16" s="101"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="98"/>
+      <c r="D16" s="85"/>
       <c r="E16" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="85"/>
+      <c r="G16" s="101"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="85"/>
-      <c r="B17" s="83"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="98"/>
+      <c r="D17" s="85"/>
       <c r="E17" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="11">
         <v>44009</v>
       </c>
-      <c r="G17" s="85"/>
+      <c r="G17" s="101"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="85"/>
-      <c r="B18" s="83"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="98"/>
+      <c r="D18" s="85"/>
       <c r="E18" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="11">
         <v>44009</v>
       </c>
-      <c r="G18" s="85"/>
+      <c r="G18" s="101"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="85"/>
-      <c r="B19" s="83"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="98"/>
+      <c r="D19" s="85"/>
       <c r="E19" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="11">
         <v>44009</v>
       </c>
-      <c r="G19" s="85"/>
+      <c r="G19" s="101"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="85"/>
-      <c r="B20" s="81"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="98"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="11">
         <v>44009</v>
       </c>
-      <c r="G20" s="85"/>
+      <c r="G20" s="101"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="85"/>
+      <c r="A21" s="101"/>
       <c r="B21" s="50" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="98"/>
+      <c r="D21" s="85"/>
       <c r="E21" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="16">
         <v>44016</v>
       </c>
-      <c r="G21" s="85"/>
+      <c r="G21" s="101"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="85"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="99"/>
+      <c r="D22" s="86"/>
       <c r="E22" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="16">
         <v>44016</v>
       </c>
-      <c r="G22" s="85"/>
+      <c r="G22" s="101"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="84">
+      <c r="A23" s="77">
         <v>2</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -2346,147 +2346,147 @@
       <c r="D23" s="55"/>
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
-      <c r="G23" s="84" t="s">
+      <c r="G23" s="77" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
-      <c r="B24" s="80" t="s">
+      <c r="A24" s="77"/>
+      <c r="B24" s="103" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="97"/>
+      <c r="D24" s="84"/>
       <c r="E24" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="16">
         <v>44010</v>
       </c>
-      <c r="G24" s="84"/>
+      <c r="G24" s="77"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
-      <c r="B25" s="83"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="98"/>
+      <c r="D25" s="85"/>
       <c r="E25" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="16">
         <v>44012</v>
       </c>
-      <c r="G25" s="84"/>
+      <c r="G25" s="77"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
-      <c r="B26" s="83"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="98"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="16">
         <v>44012</v>
       </c>
-      <c r="G26" s="84"/>
+      <c r="G26" s="77"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="83"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="98"/>
+      <c r="D27" s="85"/>
       <c r="E27" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="16"/>
-      <c r="G27" s="84"/>
+      <c r="G27" s="77"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
-      <c r="B28" s="83"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="98"/>
+      <c r="D28" s="85"/>
       <c r="E28" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="16">
         <v>44013</v>
       </c>
-      <c r="G28" s="84"/>
+      <c r="G28" s="77"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
-      <c r="B29" s="83"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="98"/>
+      <c r="D29" s="85"/>
       <c r="E29" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="16">
         <v>44015</v>
       </c>
-      <c r="G29" s="84"/>
+      <c r="G29" s="77"/>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
-      <c r="B30" s="83"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="98"/>
+      <c r="D30" s="85"/>
       <c r="E30" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="16">
         <v>44016</v>
       </c>
-      <c r="G30" s="84"/>
+      <c r="G30" s="77"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="77"/>
       <c r="B31" s="60" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="98"/>
+      <c r="D31" s="85"/>
       <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F31" s="16">
         <v>44016</v>
       </c>
-      <c r="G31" s="84"/>
+      <c r="G31" s="77"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="99"/>
+      <c r="D32" s="86"/>
       <c r="E32" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="16">
         <v>44016</v>
       </c>
-      <c r="G32" s="84"/>
+      <c r="G32" s="77"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="93">
+      <c r="A33" s="102">
         <v>3</v>
       </c>
       <c r="B33" s="21" t="s">
@@ -2498,19 +2498,19 @@
       <c r="D33" s="22"/>
       <c r="E33" s="23"/>
       <c r="F33" s="24"/>
-      <c r="G33" s="76" t="s">
+      <c r="G33" s="90" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="93"/>
-      <c r="B34" s="80" t="s">
+      <c r="A34" s="102"/>
+      <c r="B34" s="103" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="121" t="s">
+      <c r="D34" s="87" t="s">
         <v>57</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -2519,143 +2519,143 @@
       <c r="F34" s="16">
         <v>44017</v>
       </c>
-      <c r="G34" s="77"/>
+      <c r="G34" s="91"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="93"/>
-      <c r="B35" s="83"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="122"/>
+      <c r="D35" s="88"/>
       <c r="E35" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="16">
         <v>44018</v>
       </c>
-      <c r="G35" s="77"/>
+      <c r="G35" s="91"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="93"/>
-      <c r="B36" s="83"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="122"/>
+      <c r="D36" s="88"/>
       <c r="E36" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F36" s="16">
         <v>44020</v>
       </c>
-      <c r="G36" s="77"/>
+      <c r="G36" s="91"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="93"/>
-      <c r="B37" s="83"/>
+      <c r="A37" s="102"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="122"/>
+      <c r="D37" s="88"/>
       <c r="E37" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F37" s="16"/>
-      <c r="G37" s="77"/>
+      <c r="G37" s="91"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="93"/>
-      <c r="B38" s="83"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="122"/>
+      <c r="D38" s="88"/>
       <c r="E38" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F38" s="16">
         <v>44022</v>
       </c>
-      <c r="G38" s="77"/>
+      <c r="G38" s="91"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="93"/>
-      <c r="B39" s="83"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="104"/>
       <c r="C39" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="122"/>
+      <c r="D39" s="88"/>
       <c r="E39" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F39" s="16">
         <v>44022</v>
       </c>
-      <c r="G39" s="77"/>
+      <c r="G39" s="91"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="93"/>
-      <c r="B40" s="83"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="122"/>
+      <c r="D40" s="88"/>
       <c r="E40" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F40" s="16">
         <v>44022</v>
       </c>
-      <c r="G40" s="77"/>
+      <c r="G40" s="91"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="93"/>
-      <c r="B41" s="81"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="122"/>
+      <c r="D41" s="88"/>
       <c r="E41" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F41" s="16">
         <v>44023</v>
       </c>
-      <c r="G41" s="77"/>
+      <c r="G41" s="91"/>
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="93"/>
+      <c r="A42" s="102"/>
       <c r="B42" s="50" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="64"/>
-      <c r="D42" s="122"/>
+      <c r="D42" s="88"/>
       <c r="E42" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F42" s="16">
         <v>44025</v>
       </c>
-      <c r="G42" s="77"/>
+      <c r="G42" s="91"/>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="93"/>
+      <c r="A43" s="102"/>
       <c r="B43" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="5"/>
-      <c r="D43" s="123"/>
+      <c r="D43" s="89"/>
       <c r="E43" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F43" s="16">
         <v>44025</v>
       </c>
-      <c r="G43" s="78"/>
+      <c r="G43" s="92"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="86">
+      <c r="A44" s="118">
         <v>4</v>
       </c>
       <c r="B44" s="25" t="s">
@@ -2667,119 +2667,147 @@
       <c r="D44" s="26"/>
       <c r="E44" s="27"/>
       <c r="F44" s="28"/>
-      <c r="G44" s="124"/>
+      <c r="G44" s="93" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="86"/>
-      <c r="B45" s="79" t="s">
+      <c r="A45" s="118"/>
+      <c r="B45" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F45" s="16">
         <v>44025</v>
       </c>
-      <c r="G45" s="125"/>
+      <c r="G45" s="94"/>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="86"/>
-      <c r="B46" s="79"/>
+      <c r="A46" s="118"/>
+      <c r="B46" s="70"/>
       <c r="C46" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F46" s="16">
         <v>44027</v>
       </c>
-      <c r="G46" s="125"/>
+      <c r="G46" s="94"/>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="86"/>
-      <c r="B47" s="79"/>
+      <c r="A47" s="118"/>
+      <c r="B47" s="70"/>
       <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F47" s="16"/>
-      <c r="G47" s="125"/>
+      <c r="G47" s="94"/>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="86"/>
-      <c r="B48" s="79"/>
+      <c r="A48" s="118"/>
+      <c r="B48" s="70"/>
       <c r="C48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F48" s="16">
         <v>44028</v>
       </c>
-      <c r="G48" s="125"/>
+      <c r="G48" s="94"/>
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="86"/>
-      <c r="B49" s="79"/>
+      <c r="A49" s="118"/>
+      <c r="B49" s="70"/>
       <c r="C49" s="64" t="s">
         <v>61</v>
       </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F49" s="16">
         <v>44028</v>
       </c>
-      <c r="G49" s="125"/>
+      <c r="G49" s="94"/>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" s="86"/>
-      <c r="B50" s="79"/>
+      <c r="A50" s="118"/>
+      <c r="B50" s="70"/>
       <c r="C50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="125"/>
+      <c r="E50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="16">
+        <v>44029</v>
+      </c>
+      <c r="G50" s="94"/>
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A51" s="86"/>
-      <c r="B51" s="79"/>
+      <c r="A51" s="118"/>
+      <c r="B51" s="70"/>
       <c r="C51" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="61"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="125"/>
+      <c r="E51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="16">
+        <v>44029</v>
+      </c>
+      <c r="G51" s="94"/>
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="86"/>
+      <c r="A52" s="118"/>
       <c r="B52" s="50" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="125"/>
+      <c r="E52" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="16">
+        <v>44030</v>
+      </c>
+      <c r="G52" s="94"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="86"/>
+      <c r="A53" s="118"/>
       <c r="B53" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="126"/>
+      <c r="E53" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="16">
+        <v>44030</v>
+      </c>
+      <c r="G53" s="95"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="87">
+      <c r="A54" s="119">
         <v>5</v>
       </c>
       <c r="B54" s="29" t="s">
@@ -2791,11 +2819,11 @@
       <c r="D54" s="30"/>
       <c r="E54" s="31"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="127"/>
+      <c r="G54" s="96"/>
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="87"/>
-      <c r="B55" s="79" t="s">
+      <c r="A55" s="119"/>
+      <c r="B55" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -2804,54 +2832,54 @@
       <c r="D55" s="2"/>
       <c r="E55" s="4"/>
       <c r="F55" s="16"/>
-      <c r="G55" s="128"/>
+      <c r="G55" s="97"/>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="87"/>
-      <c r="B56" s="79"/>
+      <c r="A56" s="119"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
       <c r="F56" s="16"/>
-      <c r="G56" s="128"/>
+      <c r="G56" s="97"/>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="87"/>
-      <c r="B57" s="79"/>
+      <c r="A57" s="119"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="128"/>
+      <c r="G57" s="97"/>
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A58" s="87"/>
-      <c r="B58" s="79"/>
+      <c r="A58" s="119"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="4"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="128"/>
+      <c r="G58" s="97"/>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="87"/>
-      <c r="B59" s="79"/>
+      <c r="A59" s="119"/>
+      <c r="B59" s="70"/>
       <c r="C59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="4"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="128"/>
+      <c r="G59" s="97"/>
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" s="87"/>
+      <c r="A60" s="119"/>
       <c r="B60" s="50" t="s">
         <v>34</v>
       </c>
@@ -2859,10 +2887,10 @@
       <c r="D60" s="2"/>
       <c r="E60" s="4"/>
       <c r="F60" s="16"/>
-      <c r="G60" s="128"/>
+      <c r="G60" s="97"/>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" s="87"/>
+      <c r="A61" s="119"/>
       <c r="B61" s="50" t="s">
         <v>8</v>
       </c>
@@ -2870,10 +2898,10 @@
       <c r="D61" s="2"/>
       <c r="E61" s="4"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="129"/>
+      <c r="G61" s="98"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="88">
+      <c r="A62" s="120">
         <v>6</v>
       </c>
       <c r="B62" s="48" t="s">
@@ -2885,39 +2913,39 @@
       <c r="D62" s="49"/>
       <c r="E62" s="33"/>
       <c r="F62" s="34"/>
-      <c r="G62" s="115"/>
+      <c r="G62" s="78"/>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="88"/>
-      <c r="B63" s="79" t="s">
+      <c r="A63" s="120"/>
+      <c r="B63" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="4"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="116"/>
+      <c r="G63" s="79"/>
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" s="88"/>
-      <c r="B64" s="79"/>
+      <c r="A64" s="120"/>
+      <c r="B64" s="70"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="4"/>
       <c r="F64" s="16"/>
-      <c r="G64" s="116"/>
+      <c r="G64" s="79"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="88"/>
-      <c r="B65" s="79"/>
+      <c r="A65" s="120"/>
+      <c r="B65" s="70"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="4"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="116"/>
+      <c r="G65" s="79"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="88"/>
+      <c r="A66" s="120"/>
       <c r="B66" s="50" t="s">
         <v>34</v>
       </c>
@@ -2925,10 +2953,10 @@
       <c r="D66" s="2"/>
       <c r="E66" s="4"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="116"/>
+      <c r="G66" s="79"/>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A67" s="88"/>
+      <c r="A67" s="120"/>
       <c r="B67" s="50" t="s">
         <v>8</v>
       </c>
@@ -2936,10 +2964,10 @@
       <c r="D67" s="2"/>
       <c r="E67" s="4"/>
       <c r="F67" s="16"/>
-      <c r="G67" s="117"/>
+      <c r="G67" s="80"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="89">
+      <c r="A68" s="121">
         <v>6</v>
       </c>
       <c r="B68" s="35" t="s">
@@ -2949,39 +2977,39 @@
       <c r="D68" s="36"/>
       <c r="E68" s="37"/>
       <c r="F68" s="37"/>
-      <c r="G68" s="118"/>
+      <c r="G68" s="81"/>
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="89"/>
-      <c r="B69" s="79" t="s">
+      <c r="A69" s="121"/>
+      <c r="B69" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="4"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="119"/>
+      <c r="G69" s="82"/>
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A70" s="89"/>
-      <c r="B70" s="79"/>
+      <c r="A70" s="121"/>
+      <c r="B70" s="70"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="4"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="119"/>
+      <c r="G70" s="82"/>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A71" s="89"/>
-      <c r="B71" s="79"/>
+      <c r="A71" s="121"/>
+      <c r="B71" s="70"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="4"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="119"/>
+      <c r="G71" s="82"/>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="89"/>
+      <c r="A72" s="121"/>
       <c r="B72" s="50" t="s">
         <v>34</v>
       </c>
@@ -2989,10 +3017,10 @@
       <c r="D72" s="2"/>
       <c r="E72" s="4"/>
       <c r="F72" s="16"/>
-      <c r="G72" s="119"/>
+      <c r="G72" s="82"/>
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A73" s="89"/>
+      <c r="A73" s="121"/>
       <c r="B73" s="50" t="s">
         <v>8</v>
       </c>
@@ -3000,10 +3028,10 @@
       <c r="D73" s="2"/>
       <c r="E73" s="4"/>
       <c r="F73" s="16"/>
-      <c r="G73" s="120"/>
+      <c r="G73" s="83"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="90">
+      <c r="A74" s="122">
         <v>7</v>
       </c>
       <c r="B74" s="38" t="s">
@@ -3013,39 +3041,39 @@
       <c r="D74" s="39"/>
       <c r="E74" s="40"/>
       <c r="F74" s="41"/>
-      <c r="G74" s="112"/>
+      <c r="G74" s="74"/>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A75" s="90"/>
-      <c r="B75" s="79" t="s">
+      <c r="A75" s="122"/>
+      <c r="B75" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="4"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="113"/>
+      <c r="G75" s="75"/>
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A76" s="90"/>
-      <c r="B76" s="79"/>
+      <c r="A76" s="122"/>
+      <c r="B76" s="70"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="4"/>
       <c r="F76" s="16"/>
-      <c r="G76" s="113"/>
+      <c r="G76" s="75"/>
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A77" s="90"/>
-      <c r="B77" s="79"/>
+      <c r="A77" s="122"/>
+      <c r="B77" s="70"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="4"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="113"/>
+      <c r="G77" s="75"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A78" s="90"/>
+      <c r="A78" s="122"/>
       <c r="B78" s="50" t="s">
         <v>34</v>
       </c>
@@ -3053,10 +3081,10 @@
       <c r="D78" s="2"/>
       <c r="E78" s="4"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="113"/>
+      <c r="G78" s="75"/>
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A79" s="90"/>
+      <c r="A79" s="122"/>
       <c r="B79" s="50" t="s">
         <v>8</v>
       </c>
@@ -3064,10 +3092,10 @@
       <c r="D79" s="2"/>
       <c r="E79" s="4"/>
       <c r="F79" s="16"/>
-      <c r="G79" s="114"/>
+      <c r="G79" s="76"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="82">
+      <c r="A80" s="123">
         <v>8</v>
       </c>
       <c r="B80" s="42" t="s">
@@ -3077,30 +3105,30 @@
       <c r="D80" s="43"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
-      <c r="G80" s="109"/>
+      <c r="G80" s="71"/>
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A81" s="82"/>
-      <c r="B81" s="79" t="s">
+      <c r="A81" s="123"/>
+      <c r="B81" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="4"/>
       <c r="F81" s="16"/>
-      <c r="G81" s="110"/>
+      <c r="G81" s="72"/>
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A82" s="82"/>
-      <c r="B82" s="79"/>
+      <c r="A82" s="123"/>
+      <c r="B82" s="70"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="4"/>
       <c r="F82" s="16"/>
-      <c r="G82" s="110"/>
+      <c r="G82" s="72"/>
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A83" s="82"/>
+      <c r="A83" s="123"/>
       <c r="B83" s="50" t="s">
         <v>7</v>
       </c>
@@ -3108,10 +3136,10 @@
       <c r="D83" s="2"/>
       <c r="E83" s="4"/>
       <c r="F83" s="16"/>
-      <c r="G83" s="110"/>
+      <c r="G83" s="72"/>
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A84" s="82"/>
+      <c r="A84" s="123"/>
       <c r="B84" s="50" t="s">
         <v>34</v>
       </c>
@@ -3119,10 +3147,10 @@
       <c r="D84" s="2"/>
       <c r="E84" s="4"/>
       <c r="F84" s="16"/>
-      <c r="G84" s="110"/>
+      <c r="G84" s="72"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A85" s="82"/>
+      <c r="A85" s="123"/>
       <c r="B85" s="50" t="s">
         <v>8</v>
       </c>
@@ -3130,10 +3158,10 @@
       <c r="D85" s="2"/>
       <c r="E85" s="4"/>
       <c r="F85" s="16"/>
-      <c r="G85" s="111"/>
+      <c r="G85" s="73"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="85">
+      <c r="A86" s="101">
         <v>9</v>
       </c>
       <c r="B86" s="12" t="s">
@@ -3143,39 +3171,39 @@
       <c r="D86" s="13"/>
       <c r="E86" s="14"/>
       <c r="F86" s="15"/>
-      <c r="G86" s="70"/>
+      <c r="G86" s="124"/>
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A87" s="85"/>
-      <c r="B87" s="79" t="s">
+      <c r="A87" s="101"/>
+      <c r="B87" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="4"/>
       <c r="F87" s="16"/>
-      <c r="G87" s="71"/>
+      <c r="G87" s="125"/>
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A88" s="85"/>
-      <c r="B88" s="79"/>
+      <c r="A88" s="101"/>
+      <c r="B88" s="70"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="4"/>
       <c r="F88" s="16"/>
-      <c r="G88" s="71"/>
+      <c r="G88" s="125"/>
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A89" s="85"/>
-      <c r="B89" s="79"/>
+      <c r="A89" s="101"/>
+      <c r="B89" s="70"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="4"/>
       <c r="F89" s="16"/>
-      <c r="G89" s="71"/>
+      <c r="G89" s="125"/>
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A90" s="85"/>
+      <c r="A90" s="101"/>
       <c r="B90" s="50" t="s">
         <v>7</v>
       </c>
@@ -3183,10 +3211,10 @@
       <c r="D90" s="2"/>
       <c r="E90" s="4"/>
       <c r="F90" s="16"/>
-      <c r="G90" s="71"/>
+      <c r="G90" s="125"/>
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="85"/>
+      <c r="A91" s="101"/>
       <c r="B91" s="50" t="s">
         <v>34</v>
       </c>
@@ -3194,10 +3222,10 @@
       <c r="D91" s="2"/>
       <c r="E91" s="4"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="71"/>
+      <c r="G91" s="125"/>
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A92" s="85"/>
+      <c r="A92" s="101"/>
       <c r="B92" s="50" t="s">
         <v>8</v>
       </c>
@@ -3205,10 +3233,10 @@
       <c r="D92" s="2"/>
       <c r="E92" s="4"/>
       <c r="F92" s="16"/>
-      <c r="G92" s="72"/>
+      <c r="G92" s="126"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="84">
+      <c r="A93" s="77">
         <v>10</v>
       </c>
       <c r="B93" s="46" t="s">
@@ -3218,30 +3246,30 @@
       <c r="D93" s="47"/>
       <c r="E93" s="19"/>
       <c r="F93" s="20"/>
-      <c r="G93" s="73"/>
+      <c r="G93" s="127"/>
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A94" s="84"/>
-      <c r="B94" s="80" t="s">
+      <c r="A94" s="77"/>
+      <c r="B94" s="103" t="s">
         <v>32</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="4"/>
       <c r="F94" s="16"/>
-      <c r="G94" s="74"/>
+      <c r="G94" s="128"/>
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A95" s="84"/>
-      <c r="B95" s="81"/>
+      <c r="A95" s="77"/>
+      <c r="B95" s="105"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="4"/>
       <c r="F95" s="16"/>
-      <c r="G95" s="74"/>
+      <c r="G95" s="128"/>
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A96" s="84"/>
+      <c r="A96" s="77"/>
       <c r="B96" s="50" t="s">
         <v>7</v>
       </c>
@@ -3249,10 +3277,10 @@
       <c r="D96" s="2"/>
       <c r="E96" s="4"/>
       <c r="F96" s="16"/>
-      <c r="G96" s="74"/>
+      <c r="G96" s="128"/>
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A97" s="84"/>
+      <c r="A97" s="77"/>
       <c r="B97" s="50" t="s">
         <v>34</v>
       </c>
@@ -3260,10 +3288,10 @@
       <c r="D97" s="2"/>
       <c r="E97" s="4"/>
       <c r="F97" s="16"/>
-      <c r="G97" s="74"/>
+      <c r="G97" s="128"/>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A98" s="84"/>
+      <c r="A98" s="77"/>
       <c r="B98" s="50" t="s">
         <v>8</v>
       </c>
@@ -3271,10 +3299,10 @@
       <c r="D98" s="2"/>
       <c r="E98" s="4"/>
       <c r="F98" s="16"/>
-      <c r="G98" s="75"/>
+      <c r="G98" s="129"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="76">
+      <c r="A99" s="90">
         <v>11</v>
       </c>
       <c r="B99" s="21" t="s">
@@ -3284,75 +3312,75 @@
       <c r="D99" s="22"/>
       <c r="E99" s="23"/>
       <c r="F99" s="24"/>
-      <c r="G99" s="76"/>
+      <c r="G99" s="90"/>
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A100" s="77"/>
-      <c r="B100" s="83" t="s">
+      <c r="A100" s="91"/>
+      <c r="B100" s="104" t="s">
         <v>32</v>
       </c>
       <c r="C100" s="52"/>
       <c r="D100" s="52"/>
       <c r="E100" s="4"/>
       <c r="F100" s="16"/>
-      <c r="G100" s="77"/>
+      <c r="G100" s="91"/>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A101" s="77"/>
-      <c r="B101" s="83"/>
+      <c r="A101" s="91"/>
+      <c r="B101" s="104"/>
       <c r="C101" s="52"/>
       <c r="D101" s="52"/>
       <c r="E101" s="4"/>
       <c r="F101" s="16"/>
-      <c r="G101" s="77"/>
+      <c r="G101" s="91"/>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A102" s="77"/>
-      <c r="B102" s="83"/>
+      <c r="A102" s="91"/>
+      <c r="B102" s="104"/>
       <c r="C102" s="52"/>
       <c r="D102" s="52"/>
       <c r="E102" s="4"/>
       <c r="F102" s="16"/>
-      <c r="G102" s="77"/>
+      <c r="G102" s="91"/>
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A103" s="77"/>
-      <c r="B103" s="83"/>
+      <c r="A103" s="91"/>
+      <c r="B103" s="104"/>
       <c r="C103" s="52"/>
       <c r="D103" s="52"/>
       <c r="E103" s="4"/>
       <c r="F103" s="16"/>
-      <c r="G103" s="77"/>
+      <c r="G103" s="91"/>
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A104" s="77"/>
-      <c r="B104" s="83"/>
+      <c r="A104" s="91"/>
+      <c r="B104" s="104"/>
       <c r="C104" s="52"/>
       <c r="D104" s="52"/>
       <c r="E104" s="4"/>
       <c r="F104" s="16"/>
-      <c r="G104" s="77"/>
+      <c r="G104" s="91"/>
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A105" s="77"/>
-      <c r="B105" s="83"/>
+      <c r="A105" s="91"/>
+      <c r="B105" s="104"/>
       <c r="C105" s="52"/>
       <c r="D105" s="52"/>
       <c r="E105" s="4"/>
       <c r="F105" s="16"/>
-      <c r="G105" s="77"/>
+      <c r="G105" s="91"/>
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A106" s="77"/>
-      <c r="B106" s="83"/>
+      <c r="A106" s="91"/>
+      <c r="B106" s="104"/>
       <c r="C106" s="52"/>
       <c r="D106" s="52"/>
       <c r="E106" s="4"/>
       <c r="F106" s="16"/>
-      <c r="G106" s="77"/>
+      <c r="G106" s="91"/>
     </row>
     <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A107" s="77"/>
+      <c r="A107" s="91"/>
       <c r="B107" s="53" t="s">
         <v>7</v>
       </c>
@@ -3360,10 +3388,10 @@
       <c r="D107" s="2"/>
       <c r="E107" s="4"/>
       <c r="F107" s="16"/>
-      <c r="G107" s="77"/>
+      <c r="G107" s="91"/>
     </row>
     <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A108" s="77"/>
+      <c r="A108" s="91"/>
       <c r="B108" s="53" t="s">
         <v>34</v>
       </c>
@@ -3371,10 +3399,10 @@
       <c r="D108" s="2"/>
       <c r="E108" s="4"/>
       <c r="F108" s="16"/>
-      <c r="G108" s="77"/>
+      <c r="G108" s="91"/>
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A109" s="78"/>
+      <c r="A109" s="92"/>
       <c r="B109" s="53" t="s">
         <v>8</v>
       </c>
@@ -3382,11 +3410,40 @@
       <c r="D109" s="2"/>
       <c r="E109" s="4"/>
       <c r="F109" s="16"/>
-      <c r="G109" s="78"/>
+      <c r="G109" s="92"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:F6" xr:uid="{60BF8AA0-547A-4AC4-BE58-D9F0611612D0}"/>
   <mergeCells count="44">
+    <mergeCell ref="G86:G92"/>
+    <mergeCell ref="G93:G98"/>
+    <mergeCell ref="G99:G109"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="A80:A85"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="A99:A109"/>
+    <mergeCell ref="B100:B106"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="A86:A92"/>
+    <mergeCell ref="A44:A53"/>
+    <mergeCell ref="A54:A61"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="A74:A79"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A43"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="D13:D22"/>
+    <mergeCell ref="B2:G5"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G12:G22"/>
     <mergeCell ref="B69:B71"/>
     <mergeCell ref="G80:G85"/>
     <mergeCell ref="G74:G79"/>
@@ -3402,35 +3459,6 @@
     <mergeCell ref="G33:G43"/>
     <mergeCell ref="G44:G53"/>
     <mergeCell ref="G54:G61"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A43"/>
-    <mergeCell ref="B13:B20"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="D13:D22"/>
-    <mergeCell ref="B2:G5"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G12:G22"/>
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="A54:A61"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="A74:A79"/>
-    <mergeCell ref="A80:A85"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="A99:A109"/>
-    <mergeCell ref="B100:B106"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="A86:A92"/>
-    <mergeCell ref="G86:G92"/>
-    <mergeCell ref="G93:G98"/>
-    <mergeCell ref="G99:G109"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="B94:B95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>